<commit_message>
Change MLP Test - Error with POX/M resolved
</commit_message>
<xml_diff>
--- a/datasets/MLP_Validation_Dataset.xlsx
+++ b/datasets/MLP_Validation_Dataset.xlsx
@@ -34,13 +34,13 @@
     <t>Mn</t>
   </si>
   <si>
-    <t>MLP_X</t>
+    <t>MLP_POX/C</t>
   </si>
   <si>
-    <t>MLP_PDI</t>
+    <t>MLP_C/A</t>
   </si>
   <si>
-    <t>MLP_Mn</t>
+    <t>MLP_POX/M</t>
   </si>
 </sst>
 </file>
@@ -453,13 +453,13 @@
         <v>81538.50378104943</v>
       </c>
       <c r="G2">
-        <v>0.6895250678062439</v>
+        <v>103.0814208984375</v>
       </c>
       <c r="H2">
-        <v>1.031888246536255</v>
+        <v>0.1061172932386398</v>
       </c>
       <c r="I2">
-        <v>81537.765625</v>
+        <v>0.0009269907604902983</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -482,13 +482,13 @@
         <v>74465.41067907</v>
       </c>
       <c r="G3">
-        <v>0.7284013628959656</v>
+        <v>107.4024810791016</v>
       </c>
       <c r="H3">
-        <v>1.033023834228516</v>
+        <v>0.09146071970462799</v>
       </c>
       <c r="I3">
-        <v>74504.6953125</v>
+        <v>0.001076534041203558</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -511,13 +511,13 @@
         <v>78830.50808908061</v>
       </c>
       <c r="G4">
-        <v>0.6867114901542664</v>
+        <v>104.7058715820312</v>
       </c>
       <c r="H4">
-        <v>1.031518816947937</v>
+        <v>0.1087210476398468</v>
       </c>
       <c r="I4">
-        <v>78864.78125</v>
+        <v>0.0009532235562801361</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -540,13 +540,13 @@
         <v>82841.31125921379</v>
       </c>
       <c r="G5">
-        <v>0.6677705645561218</v>
+        <v>112.2057723999023</v>
       </c>
       <c r="H5">
-        <v>1.031142234802246</v>
+        <v>0.1103779003024101</v>
       </c>
       <c r="I5">
-        <v>82696.9609375</v>
+        <v>0.000877119367942214</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -569,13 +569,13 @@
         <v>96695.83683405023</v>
       </c>
       <c r="G6">
-        <v>0.7113516330718994</v>
+        <v>98.08292388916016</v>
       </c>
       <c r="H6">
-        <v>1.034701347351074</v>
+        <v>0.08956778794527054</v>
       </c>
       <c r="I6">
-        <v>95012.296875</v>
+        <v>0.0008009832235984504</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -598,13 +598,13 @@
         <v>89221.94783598969</v>
       </c>
       <c r="G7">
-        <v>0.6794846653938293</v>
+        <v>110.3029937744141</v>
       </c>
       <c r="H7">
-        <v>1.032262086868286</v>
+        <v>0.1010441407561302</v>
       </c>
       <c r="I7">
-        <v>88738.421875</v>
+        <v>0.0008288382086902857</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -627,13 +627,13 @@
         <v>73551.88058884651</v>
       </c>
       <c r="G8">
-        <v>0.715279221534729</v>
+        <v>97.52388763427734</v>
       </c>
       <c r="H8">
-        <v>1.032357096672058</v>
+        <v>0.1034720614552498</v>
       </c>
       <c r="I8">
-        <v>73560.3046875</v>
+        <v>0.001071680919267237</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -656,13 +656,13 @@
         <v>76427.09527010556</v>
       </c>
       <c r="G9">
-        <v>0.6883814334869385</v>
+        <v>116.1031188964844</v>
       </c>
       <c r="H9">
-        <v>1.031572103500366</v>
+        <v>0.1017512157559395</v>
       </c>
       <c r="I9">
-        <v>76505.609375</v>
+        <v>0.0009811542695388198</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -685,13 +685,13 @@
         <v>77261.85062254904</v>
       </c>
       <c r="G10">
-        <v>0.7147232294082642</v>
+        <v>94.48360443115234</v>
       </c>
       <c r="H10">
-        <v>1.03279173374176</v>
+        <v>0.1032285764813423</v>
       </c>
       <c r="I10">
-        <v>77370.765625</v>
+        <v>0.001019283314235508</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -714,13 +714,13 @@
         <v>66432.29719207993</v>
       </c>
       <c r="G11">
-        <v>0.7007717490196228</v>
+        <v>107.8821487426758</v>
       </c>
       <c r="H11">
-        <v>1.031077146530151</v>
+        <v>0.1095517128705978</v>
       </c>
       <c r="I11">
-        <v>66636.71875</v>
+        <v>0.001142190187238157</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -743,13 +743,13 @@
         <v>66425.55258270158</v>
       </c>
       <c r="G12">
-        <v>0.7223302721977234</v>
+        <v>107.6441802978516</v>
       </c>
       <c r="H12">
-        <v>1.031853675842285</v>
+        <v>0.09948558360338211</v>
       </c>
       <c r="I12">
-        <v>66568.234375</v>
+        <v>0.001181523548439145</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -772,13 +772,13 @@
         <v>82897.20479325813</v>
       </c>
       <c r="G13">
-        <v>0.6761585474014282</v>
+        <v>104.6858444213867</v>
       </c>
       <c r="H13">
-        <v>1.031453132629395</v>
+        <v>0.1108664721250534</v>
       </c>
       <c r="I13">
-        <v>82777.8984375</v>
+        <v>0.0008913784986361861</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -801,13 +801,13 @@
         <v>72324.81594804979</v>
       </c>
       <c r="G14">
-        <v>0.7024824023246765</v>
+        <v>105.0157089233398</v>
       </c>
       <c r="H14">
-        <v>1.03151524066925</v>
+        <v>0.1063582599163055</v>
       </c>
       <c r="I14">
-        <v>72326.796875</v>
+        <v>0.001063936273567379</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -830,13 +830,13 @@
         <v>83935.62639688494</v>
       </c>
       <c r="G15">
-        <v>0.6965533494949341</v>
+        <v>107.9702453613281</v>
       </c>
       <c r="H15">
-        <v>1.032730937004089</v>
+        <v>0.09786266833543777</v>
       </c>
       <c r="I15">
-        <v>83995.3359375</v>
+        <v>0.0009142440976575017</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -859,13 +859,13 @@
         <v>93837.49906414766</v>
       </c>
       <c r="G16">
-        <v>0.6906330585479736</v>
+        <v>106.8684234619141</v>
       </c>
       <c r="H16">
-        <v>1.033448338508606</v>
+        <v>0.09507674723863602</v>
       </c>
       <c r="I16">
-        <v>92288.40625</v>
+        <v>0.0008000473026186228</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -888,13 +888,13 @@
         <v>75377.83846040601</v>
       </c>
       <c r="G17">
-        <v>0.7433887720108032</v>
+        <v>77.248291015625</v>
       </c>
       <c r="H17">
-        <v>1.035325407981873</v>
+        <v>0.09991727024316788</v>
       </c>
       <c r="I17">
-        <v>75599.40625</v>
+        <v>0.001102535519748926</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -917,13 +917,13 @@
         <v>83429.7766818427</v>
       </c>
       <c r="G18">
-        <v>0.7006247043609619</v>
+        <v>90.19596099853516</v>
       </c>
       <c r="H18">
-        <v>1.033215761184692</v>
+        <v>0.1077146530151367</v>
       </c>
       <c r="I18">
-        <v>83222.34375</v>
+        <v>0.0009344257996417582</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -946,13 +946,13 @@
         <v>78495.33357414858</v>
       </c>
       <c r="G19">
-        <v>0.6866658329963684</v>
+        <v>115.9886322021484</v>
       </c>
       <c r="H19">
-        <v>1.031671524047852</v>
+        <v>0.1007870212197304</v>
       </c>
       <c r="I19">
-        <v>78538.1015625</v>
+        <v>0.0009542822372168303</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -975,13 +975,13 @@
         <v>71426.37757296051</v>
       </c>
       <c r="G20">
-        <v>0.6804216504096985</v>
+        <v>119.8404922485352</v>
       </c>
       <c r="H20">
-        <v>1.030719041824341</v>
+        <v>0.1078280135989189</v>
       </c>
       <c r="I20">
-        <v>71652.7421875</v>
+        <v>0.00102788454387337</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1004,13 +1004,13 @@
         <v>67280.96655030428</v>
       </c>
       <c r="G21">
-        <v>0.6976336240768433</v>
+        <v>110.2782592773438</v>
       </c>
       <c r="H21">
-        <v>1.030939340591431</v>
+        <v>0.1088702753186226</v>
       </c>
       <c r="I21">
-        <v>67343.0390625</v>
+        <v>0.001124369795434177</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1033,13 +1033,13 @@
         <v>70626.40064168505</v>
       </c>
       <c r="G22">
-        <v>0.6834704875946045</v>
+        <v>123.5957412719727</v>
       </c>
       <c r="H22">
-        <v>1.030915141105652</v>
+        <v>0.1036246493458748</v>
       </c>
       <c r="I22">
-        <v>70867.5546875</v>
+        <v>0.00104227545671165</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1062,13 +1062,13 @@
         <v>68248.14291811716</v>
       </c>
       <c r="G23">
-        <v>0.7146124839782715</v>
+        <v>103.6113510131836</v>
       </c>
       <c r="H23">
-        <v>1.031673312187195</v>
+        <v>0.1043815985321999</v>
       </c>
       <c r="I23">
-        <v>68295.125</v>
+        <v>0.001144745154306293</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1091,13 +1091,13 @@
         <v>80811.52741395582</v>
       </c>
       <c r="G24">
-        <v>0.6754887104034424</v>
+        <v>104.5465774536133</v>
       </c>
       <c r="H24">
-        <v>1.031241297721863</v>
+        <v>0.1128630265593529</v>
       </c>
       <c r="I24">
-        <v>80702.1015625</v>
+        <v>0.0009147664532065392</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1120,13 +1120,13 @@
         <v>68738.83122165086</v>
       </c>
       <c r="G25">
-        <v>0.7029218673706055</v>
+        <v>105.777473449707</v>
       </c>
       <c r="H25">
-        <v>1.031219840049744</v>
+        <v>0.1084329858422279</v>
       </c>
       <c r="I25">
-        <v>68763.2890625</v>
+        <v>0.00111474480945617</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1149,13 +1149,13 @@
         <v>91637.49349395366</v>
       </c>
       <c r="G26">
-        <v>0.7210232615470886</v>
+        <v>83.69991302490234</v>
       </c>
       <c r="H26">
-        <v>1.035190343856812</v>
+        <v>0.09746511280536652</v>
       </c>
       <c r="I26">
-        <v>90744.6796875</v>
+        <v>0.0008741109049879014</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1178,13 +1178,13 @@
         <v>66606.44255704015</v>
       </c>
       <c r="G27">
-        <v>0.7153734564781189</v>
+        <v>105.2832107543945</v>
       </c>
       <c r="H27">
-        <v>1.03155505657196</v>
+        <v>0.1040679067373276</v>
       </c>
       <c r="I27">
-        <v>66662.34375</v>
+        <v>0.001169332186691463</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1207,13 +1207,13 @@
         <v>80737.07906334888</v>
       </c>
       <c r="G28">
-        <v>0.7645170092582703</v>
+        <v>69.32630920410156</v>
       </c>
       <c r="H28">
-        <v>1.037353277206421</v>
+        <v>0.09002368152141571</v>
       </c>
       <c r="I28">
-        <v>80620.2890625</v>
+        <v>0.001087538781575859</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1236,13 +1236,13 @@
         <v>85125.14020514555</v>
       </c>
       <c r="G29">
-        <v>0.6928711533546448</v>
+        <v>112.7721862792969</v>
       </c>
       <c r="H29">
-        <v>1.032721519470215</v>
+        <v>0.09546726942062378</v>
       </c>
       <c r="I29">
-        <v>85159.734375</v>
+        <v>0.0008973635849542916</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1265,13 +1265,13 @@
         <v>66848.48321000017</v>
       </c>
       <c r="G30">
-        <v>0.7156188488006592</v>
+        <v>101.2170104980469</v>
       </c>
       <c r="H30">
-        <v>1.031666159629822</v>
+        <v>0.1061341241002083</v>
       </c>
       <c r="I30">
-        <v>66908.1484375</v>
+        <v>0.001167446607723832</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1294,13 +1294,13 @@
         <v>75157.52364805204</v>
       </c>
       <c r="G31">
-        <v>0.7390630841255188</v>
+        <v>96.56613159179688</v>
       </c>
       <c r="H31">
-        <v>1.034109711647034</v>
+        <v>0.09197403490543365</v>
       </c>
       <c r="I31">
-        <v>75200.7890625</v>
+        <v>0.001091325888410211</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1323,13 +1323,13 @@
         <v>86032.53825126126</v>
       </c>
       <c r="G32">
-        <v>0.7040819525718689</v>
+        <v>97.45156097412109</v>
       </c>
       <c r="H32">
-        <v>1.033243656158447</v>
+        <v>0.09990600496530533</v>
       </c>
       <c r="I32">
-        <v>85951.625</v>
+        <v>0.0009015981340780854</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1352,13 +1352,13 @@
         <v>85143.38850386722</v>
       </c>
       <c r="G33">
-        <v>0.6909925937652588</v>
+        <v>111.1525039672852</v>
       </c>
       <c r="H33">
-        <v>1.032472848892212</v>
+        <v>0.09747848659753799</v>
       </c>
       <c r="I33">
-        <v>85106.7421875</v>
+        <v>0.0008931300835683942</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1381,13 +1381,13 @@
         <v>81924.5274006101</v>
       </c>
       <c r="G34">
-        <v>0.7415155172348022</v>
+        <v>97.54296875</v>
       </c>
       <c r="H34">
-        <v>1.035019755363464</v>
+        <v>0.08591195195913315</v>
       </c>
       <c r="I34">
-        <v>81812.09375</v>
+        <v>0.001010555773973465</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1410,13 +1410,13 @@
         <v>94595.76326410174</v>
       </c>
       <c r="G35">
-        <v>0.7005072832107544</v>
+        <v>98.82180786132812</v>
       </c>
       <c r="H35">
-        <v>1.033807635307312</v>
+        <v>0.09542214870452881</v>
       </c>
       <c r="I35">
-        <v>93437.859375</v>
+        <v>0.0008078051614575088</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1439,13 +1439,13 @@
         <v>90149.4161812352</v>
       </c>
       <c r="G36">
-        <v>0.7165442109107971</v>
+        <v>79.54354095458984</v>
       </c>
       <c r="H36">
-        <v>1.034945726394653</v>
+        <v>0.1028676852583885</v>
       </c>
       <c r="I36">
-        <v>89415.5703125</v>
+        <v>0.0008844593539834023</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1468,13 +1468,13 @@
         <v>78777.28742279726</v>
       </c>
       <c r="G37">
-        <v>0.6975511908531189</v>
+        <v>103.3272247314453</v>
       </c>
       <c r="H37">
-        <v>1.031975626945496</v>
+        <v>0.104409471154213</v>
       </c>
       <c r="I37">
-        <v>78759.4765625</v>
+        <v>0.0009699240908958018</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1497,13 +1497,13 @@
         <v>80320.57700922184</v>
       </c>
       <c r="G38">
-        <v>0.6964130401611328</v>
+        <v>103.4603881835938</v>
       </c>
       <c r="H38">
-        <v>1.032090663909912</v>
+        <v>0.103514738380909</v>
       </c>
       <c r="I38">
-        <v>80314.359375</v>
+        <v>0.0009503204491920769</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1526,13 +1526,13 @@
         <v>77213.73242142811</v>
       </c>
       <c r="G39">
-        <v>0.6953240633010864</v>
+        <v>104.730110168457</v>
       </c>
       <c r="H39">
-        <v>1.031713366508484</v>
+        <v>0.1060795411467552</v>
       </c>
       <c r="I39">
-        <v>77208.2578125</v>
+        <v>0.0009856425458565354</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1555,13 +1555,13 @@
         <v>79846.95430622832</v>
       </c>
       <c r="G40">
-        <v>0.6724802255630493</v>
+        <v>131.4945526123047</v>
       </c>
       <c r="H40">
-        <v>1.031446576118469</v>
+        <v>0.09428154677152634</v>
       </c>
       <c r="I40">
-        <v>80084.4140625</v>
+        <v>0.0009167870157398283</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1584,13 +1584,13 @@
         <v>75743.91139820353</v>
       </c>
       <c r="G41">
-        <v>0.7134528160095215</v>
+        <v>105.2180557250977</v>
       </c>
       <c r="H41">
-        <v>1.032387495040894</v>
+        <v>0.09834965318441391</v>
       </c>
       <c r="I41">
-        <v>75729.203125</v>
+        <v>0.001033710315823555</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1613,13 +1613,13 @@
         <v>67592.10765335572</v>
       </c>
       <c r="G42">
-        <v>0.7040764093399048</v>
+        <v>105.0943222045898</v>
       </c>
       <c r="H42">
-        <v>1.031346917152405</v>
+        <v>0.1088519617915154</v>
       </c>
       <c r="I42">
-        <v>67734.9921875</v>
+        <v>0.001134396996349096</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1642,13 +1642,13 @@
         <v>91755.36511022542</v>
       </c>
       <c r="G43">
-        <v>0.7067130208015442</v>
+        <v>98.07933044433594</v>
       </c>
       <c r="H43">
-        <v>1.033879041671753</v>
+        <v>0.09460529685020447</v>
       </c>
       <c r="I43">
-        <v>91149.1953125</v>
+        <v>0.0008455225033685565</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1671,13 +1671,13 @@
         <v>77311.84171533454</v>
       </c>
       <c r="G44">
-        <v>0.7093775868415833</v>
+        <v>104.1014556884766</v>
       </c>
       <c r="H44">
-        <v>1.032374262809753</v>
+        <v>0.09968871623277664</v>
       </c>
       <c r="I44">
-        <v>77288.3828125</v>
+        <v>0.001007793936878443</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1700,13 +1700,13 @@
         <v>89129.26059555032</v>
       </c>
       <c r="G45">
-        <v>0.6909629702568054</v>
+        <v>110.1718826293945</v>
       </c>
       <c r="H45">
-        <v>1.033080339431763</v>
+        <v>0.09491527080535889</v>
       </c>
       <c r="I45">
-        <v>88369.2578125</v>
+        <v>0.0008518586400896311</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1729,13 +1729,13 @@
         <v>69787.83105223658</v>
       </c>
       <c r="G46">
-        <v>0.6939576268196106</v>
+        <v>107.2910308837891</v>
       </c>
       <c r="H46">
-        <v>1.030947089195251</v>
+        <v>0.1113308370113373</v>
       </c>
       <c r="I46">
-        <v>69871.53125</v>
+        <v>0.001081686117686331</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1758,13 +1758,13 @@
         <v>78161.3104917923</v>
       </c>
       <c r="G47">
-        <v>0.6865009069442749</v>
+        <v>107.7700958251953</v>
       </c>
       <c r="H47">
-        <v>1.031488299369812</v>
+        <v>0.107299767434597</v>
       </c>
       <c r="I47">
-        <v>78213.5625</v>
+        <v>0.0009591238340362906</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1787,13 +1787,13 @@
         <v>82694.22254685163</v>
       </c>
       <c r="G48">
-        <v>0.7538259029388428</v>
+        <v>81.1357421875</v>
       </c>
       <c r="H48">
-        <v>1.036533713340759</v>
+        <v>0.08826431632041931</v>
       </c>
       <c r="I48">
-        <v>82460.6171875</v>
+        <v>0.001037289504893124</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1816,13 +1816,13 @@
         <v>86541.90034558781</v>
       </c>
       <c r="G49">
-        <v>0.6881836652755737</v>
+        <v>112.0285949707031</v>
       </c>
       <c r="H49">
-        <v>1.032581806182861</v>
+        <v>0.09677829593420029</v>
       </c>
       <c r="I49">
-        <v>86047.0390625</v>
+        <v>0.0008743823855184019</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1845,13 +1845,13 @@
         <v>88164.86777930609</v>
       </c>
       <c r="G50">
-        <v>0.6903793811798096</v>
+        <v>103.6875610351562</v>
       </c>
       <c r="H50">
-        <v>1.032633543014526</v>
+        <v>0.100450336933136</v>
       </c>
       <c r="I50">
-        <v>87768.0078125</v>
+        <v>0.0008556102402508259</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1874,13 +1874,13 @@
         <v>75383.59993599266</v>
       </c>
       <c r="G51">
-        <v>0.6854066848754883</v>
+        <v>105.5441131591797</v>
       </c>
       <c r="H51">
-        <v>1.031194925308228</v>
+        <v>0.1119841933250427</v>
       </c>
       <c r="I51">
-        <v>75475.21875</v>
+        <v>0.0009930119849741459</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1903,13 +1903,13 @@
         <v>85600.81365638027</v>
       </c>
       <c r="G52">
-        <v>0.7290211915969849</v>
+        <v>112.0933151245117</v>
       </c>
       <c r="H52">
-        <v>1.034503579139709</v>
+        <v>0.08106516301631927</v>
       </c>
       <c r="I52">
-        <v>85512.40625</v>
+        <v>0.0009430547943338752</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1932,13 +1932,13 @@
         <v>65890.78658717666</v>
       </c>
       <c r="G53">
-        <v>0.7050864100456238</v>
+        <v>105.3969802856445</v>
       </c>
       <c r="H53">
-        <v>1.031169176101685</v>
+        <v>0.1095593497157097</v>
       </c>
       <c r="I53">
-        <v>66026.5625</v>
+        <v>0.00115859997458756</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -1961,13 +1961,13 @@
         <v>72479.6296109854</v>
       </c>
       <c r="G54">
-        <v>0.7282907962799072</v>
+        <v>102.931510925293</v>
       </c>
       <c r="H54">
-        <v>1.032879710197449</v>
+        <v>0.0949527695775032</v>
       </c>
       <c r="I54">
-        <v>72590.2421875</v>
+        <v>0.001105818897485733</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -1990,13 +1990,13 @@
         <v>73602.51374138611</v>
       </c>
       <c r="G55">
-        <v>0.7279511094093323</v>
+        <v>81.80760955810547</v>
       </c>
       <c r="H55">
-        <v>1.033893585205078</v>
+        <v>0.1061497703194618</v>
       </c>
       <c r="I55">
-        <v>73597.6875</v>
+        <v>0.00109031330794096</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2019,13 +2019,13 @@
         <v>73883.31084644256</v>
       </c>
       <c r="G56">
-        <v>0.7611542344093323</v>
+        <v>78.31877136230469</v>
       </c>
       <c r="H56">
-        <v>1.036199688911438</v>
+        <v>0.09139369428157806</v>
       </c>
       <c r="I56">
-        <v>74363.25</v>
+        <v>0.00115877203643322</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2048,13 +2048,13 @@
         <v>90324.24573556196</v>
       </c>
       <c r="G57">
-        <v>0.686964213848114</v>
+        <v>108.5542297363281</v>
       </c>
       <c r="H57">
-        <v>1.032801389694214</v>
+        <v>0.09710882604122162</v>
       </c>
       <c r="I57">
-        <v>89435.8359375</v>
+        <v>0.0008292864076793194</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2077,13 +2077,13 @@
         <v>73545.58559935106</v>
       </c>
       <c r="G58">
-        <v>0.688066303730011</v>
+        <v>108.451789855957</v>
       </c>
       <c r="H58">
-        <v>1.031083464622498</v>
+        <v>0.1106163859367371</v>
       </c>
       <c r="I58">
-        <v>73624.4296875</v>
+        <v>0.001018034876324236</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2106,13 +2106,13 @@
         <v>77169.51657621456</v>
       </c>
       <c r="G59">
-        <v>0.7206875681877136</v>
+        <v>90.52240753173828</v>
       </c>
       <c r="H59">
-        <v>1.033377766609192</v>
+        <v>0.1024210229516029</v>
       </c>
       <c r="I59">
-        <v>77121.1015625</v>
+        <v>0.001032955595292151</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2135,13 +2135,13 @@
         <v>68775.78930627124</v>
       </c>
       <c r="G60">
-        <v>0.7350211143493652</v>
+        <v>98.63609313964844</v>
       </c>
       <c r="H60">
-        <v>1.033065319061279</v>
+        <v>0.09650558233261108</v>
       </c>
       <c r="I60">
-        <v>68965.5625</v>
+        <v>0.001168338232673705</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2164,13 +2164,13 @@
         <v>91194.44193383394</v>
       </c>
       <c r="G61">
-        <v>0.7451061606407166</v>
+        <v>81.74549102783203</v>
       </c>
       <c r="H61">
-        <v>1.036655068397522</v>
+        <v>0.08736676722764969</v>
       </c>
       <c r="I61">
-        <v>90037.703125</v>
+        <v>0.0009168879478238523</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2193,13 +2193,13 @@
         <v>86528.84316365354</v>
       </c>
       <c r="G62">
-        <v>0.7031577229499817</v>
+        <v>93.93820953369141</v>
       </c>
       <c r="H62">
-        <v>1.033405184745789</v>
+        <v>0.1024111583828926</v>
       </c>
       <c r="I62">
-        <v>86343.265625</v>
+        <v>0.0008966950117610395</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2222,13 +2222,13 @@
         <v>94447.96306783588</v>
       </c>
       <c r="G63">
-        <v>0.7152944803237915</v>
+        <v>84.73322296142578</v>
       </c>
       <c r="H63">
-        <v>1.035075306892395</v>
+        <v>0.09701880812644958</v>
       </c>
       <c r="I63">
-        <v>92991.890625</v>
+        <v>0.0008423365070484579</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2251,13 +2251,13 @@
         <v>89276.023230689</v>
       </c>
       <c r="G64">
-        <v>0.667989194393158</v>
+        <v>119.7322387695312</v>
       </c>
       <c r="H64">
-        <v>1.031788945198059</v>
+        <v>0.1004076153039932</v>
       </c>
       <c r="I64">
-        <v>88637.9609375</v>
+        <v>0.0008070744224824011</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2280,13 +2280,13 @@
         <v>67492.02658628208</v>
       </c>
       <c r="G65">
-        <v>0.7149878740310669</v>
+        <v>84.86528778076172</v>
       </c>
       <c r="H65">
-        <v>1.032370924949646</v>
+        <v>0.1141278669238091</v>
       </c>
       <c r="I65">
-        <v>67499.734375</v>
+        <v>0.001156971091404557</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2309,13 +2309,13 @@
         <v>72120.84373442782</v>
       </c>
       <c r="G66">
-        <v>0.6996127963066101</v>
+        <v>106.0257415771484</v>
       </c>
       <c r="H66">
-        <v>1.031735897064209</v>
+        <v>0.1071436703205109</v>
       </c>
       <c r="I66">
-        <v>72185.40625</v>
+        <v>0.001061986200511456</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2338,13 +2338,13 @@
         <v>69491.07525294257</v>
       </c>
       <c r="G67">
-        <v>0.7040020823478699</v>
+        <v>105.4516754150391</v>
       </c>
       <c r="H67">
-        <v>1.031481146812439</v>
+        <v>0.1073522865772247</v>
       </c>
       <c r="I67">
-        <v>69598.2421875</v>
+        <v>0.001107891439460218</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2367,13 +2367,13 @@
         <v>87566.73374752047</v>
       </c>
       <c r="G68">
-        <v>0.7240529656410217</v>
+        <v>99.50115966796875</v>
       </c>
       <c r="H68">
-        <v>1.034438490867615</v>
+        <v>0.08859168738126755</v>
       </c>
       <c r="I68">
-        <v>87230.1796875</v>
+        <v>0.0009181066416203976</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2396,13 +2396,13 @@
         <v>80099.88371637101</v>
       </c>
       <c r="G69">
-        <v>0.7408505082130432</v>
+        <v>79.49641418457031</v>
       </c>
       <c r="H69">
-        <v>1.035601854324341</v>
+        <v>0.09738478809595108</v>
       </c>
       <c r="I69">
-        <v>80090.25</v>
+        <v>0.001040427829138935</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2425,13 +2425,13 @@
         <v>86055.46884267239</v>
       </c>
       <c r="G70">
-        <v>0.6620885729789734</v>
+        <v>137.3601684570312</v>
       </c>
       <c r="H70">
-        <v>1.031504511833191</v>
+        <v>0.09140300005674362</v>
       </c>
       <c r="I70">
-        <v>86008.21875</v>
+        <v>0.0008292579441331327</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2454,13 +2454,13 @@
         <v>85011.69015755533</v>
       </c>
       <c r="G71">
-        <v>0.75043123960495</v>
+        <v>73.88394927978516</v>
       </c>
       <c r="H71">
-        <v>1.03681480884552</v>
+        <v>0.09292391687631607</v>
       </c>
       <c r="I71">
-        <v>84627.8046875</v>
+        <v>0.001006413018330932</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2483,13 +2483,13 @@
         <v>65295.51843847329</v>
       </c>
       <c r="G72">
-        <v>0.710395336151123</v>
+        <v>100.3096389770508</v>
       </c>
       <c r="H72">
-        <v>1.031302690505981</v>
+        <v>0.1103391945362091</v>
       </c>
       <c r="I72">
-        <v>65357.890625</v>
+        <v>0.001180648221634328</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -2512,13 +2512,13 @@
         <v>73809.16535697946</v>
       </c>
       <c r="G73">
-        <v>0.7576285004615784</v>
+        <v>95.18865966796875</v>
       </c>
       <c r="H73">
-        <v>1.035253882408142</v>
+        <v>0.08438589423894882</v>
       </c>
       <c r="I73">
-        <v>74117.1015625</v>
+        <v>0.001144233625382185</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -2541,13 +2541,13 @@
         <v>82545.26761393597</v>
       </c>
       <c r="G74">
-        <v>0.7056410312652588</v>
+        <v>91.97579193115234</v>
       </c>
       <c r="H74">
-        <v>1.033029794692993</v>
+        <v>0.1055807843804359</v>
       </c>
       <c r="I74">
-        <v>82681.3046875</v>
+        <v>0.0009469838696531951</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -2570,13 +2570,13 @@
         <v>71623.59727313645</v>
       </c>
       <c r="G75">
-        <v>0.7580825090408325</v>
+        <v>100.6641464233398</v>
       </c>
       <c r="H75">
-        <v>1.034785032272339</v>
+        <v>0.08234095573425293</v>
       </c>
       <c r="I75">
-        <v>72108.7421875</v>
+        <v>0.001171366078779101</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -2599,13 +2599,13 @@
         <v>81320.40426984521</v>
       </c>
       <c r="G76">
-        <v>0.6705456972122192</v>
+        <v>122.6593475341797</v>
       </c>
       <c r="H76">
-        <v>1.031268000602722</v>
+        <v>0.1019734442234039</v>
       </c>
       <c r="I76">
-        <v>81460.125</v>
+        <v>0.0008979855920188129</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -2628,13 +2628,13 @@
         <v>72790.46354393325</v>
       </c>
       <c r="G77">
-        <v>0.7603940963745117</v>
+        <v>64.06911468505859</v>
       </c>
       <c r="H77">
-        <v>1.03657603263855</v>
+        <v>0.09990126639604568</v>
       </c>
       <c r="I77">
-        <v>73545.9453125</v>
+        <v>0.001172894961200655</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -2657,13 +2657,13 @@
         <v>70608.55581957518</v>
       </c>
       <c r="G78">
-        <v>0.7448294758796692</v>
+        <v>89.03109741210938</v>
       </c>
       <c r="H78">
-        <v>1.034352779388428</v>
+        <v>0.09614625573158264</v>
       </c>
       <c r="I78">
-        <v>70918.2578125</v>
+        <v>0.001165261841379106</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -2686,13 +2686,13 @@
         <v>69925.81047232136</v>
       </c>
       <c r="G79">
-        <v>0.7087756991386414</v>
+        <v>87.67147064208984</v>
       </c>
       <c r="H79">
-        <v>1.032222747802734</v>
+        <v>0.1141339614987373</v>
       </c>
       <c r="I79">
-        <v>69914.3984375</v>
+        <v>0.001110714045353234</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -2715,13 +2715,13 @@
         <v>74599.91229194535</v>
       </c>
       <c r="G80">
-        <v>0.711596667766571</v>
+        <v>92.44651794433594</v>
       </c>
       <c r="H80">
-        <v>1.032447934150696</v>
+        <v>0.1073962822556496</v>
       </c>
       <c r="I80">
-        <v>74604.6640625</v>
+        <v>0.001050759572535753</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -2744,13 +2744,13 @@
         <v>76030.25181731302</v>
       </c>
       <c r="G81">
-        <v>0.7688736915588379</v>
+        <v>64.65254974365234</v>
       </c>
       <c r="H81">
-        <v>1.037323474884033</v>
+        <v>0.09311513602733612</v>
       </c>
       <c r="I81">
-        <v>76459.0234375</v>
+        <v>0.001149710267782211</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -2773,13 +2773,13 @@
         <v>89345.48785304721</v>
       </c>
       <c r="G82">
-        <v>0.7357191443443298</v>
+        <v>91.00156402587891</v>
       </c>
       <c r="H82">
-        <v>1.03565526008606</v>
+        <v>0.08767616003751755</v>
       </c>
       <c r="I82">
-        <v>88787.8984375</v>
+        <v>0.0009154428262263536</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -2802,13 +2802,13 @@
         <v>69659.94878883265</v>
       </c>
       <c r="G83">
-        <v>0.719272792339325</v>
+        <v>96.16300964355469</v>
       </c>
       <c r="H83">
-        <v>1.032247185707092</v>
+        <v>0.1046929955482483</v>
       </c>
       <c r="I83">
-        <v>69691.546875</v>
+        <v>0.001133369514718652</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -2831,13 +2831,13 @@
         <v>77414.34810601255</v>
       </c>
       <c r="G84">
-        <v>0.7282801270484924</v>
+        <v>80.141845703125</v>
       </c>
       <c r="H84">
-        <v>1.034441709518433</v>
+        <v>0.1043293550610542</v>
       </c>
       <c r="I84">
-        <v>77399.578125</v>
+        <v>0.001042614807374775</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -2860,13 +2860,13 @@
         <v>94602.86908759469</v>
       </c>
       <c r="G85">
-        <v>0.6983616352081299</v>
+        <v>98.56911468505859</v>
       </c>
       <c r="H85">
-        <v>1.033726572990417</v>
+        <v>0.09683864563703537</v>
       </c>
       <c r="I85">
-        <v>93436.03125</v>
+        <v>0.0008028442389331758</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -2889,13 +2889,13 @@
         <v>78210.63072795217</v>
       </c>
       <c r="G86">
-        <v>0.6755329966545105</v>
+        <v>108.6180725097656</v>
       </c>
       <c r="H86">
-        <v>1.031030058860779</v>
+        <v>0.1123553365468979</v>
       </c>
       <c r="I86">
-        <v>78294.7890625</v>
+        <v>0.0009420947171747684</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -2918,13 +2918,13 @@
         <v>89517.44737723017</v>
       </c>
       <c r="G87">
-        <v>0.6993902325630188</v>
+        <v>99.50419616699219</v>
       </c>
       <c r="H87">
-        <v>1.033323526382446</v>
+        <v>0.09823919087648392</v>
       </c>
       <c r="I87">
-        <v>89083.7890625</v>
+        <v>0.0008593962993472815</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -2947,13 +2947,13 @@
         <v>67099.66344767701</v>
       </c>
       <c r="G88">
-        <v>0.7248297929763794</v>
+        <v>101.0179901123047</v>
       </c>
       <c r="H88">
-        <v>1.032199263572693</v>
+        <v>0.1012815311551094</v>
       </c>
       <c r="I88">
-        <v>67215.4921875</v>
+        <v>0.001177631318569183</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -2976,13 +2976,13 @@
         <v>80887.51816786182</v>
       </c>
       <c r="G89">
-        <v>0.7220001220703125</v>
+        <v>83.19351959228516</v>
       </c>
       <c r="H89">
-        <v>1.034262299537659</v>
+        <v>0.1038530021905899</v>
       </c>
       <c r="I89">
-        <v>80871.34375</v>
+        <v>0.0009889275534078479</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3005,13 +3005,13 @@
         <v>75969.34526755988</v>
       </c>
       <c r="G90">
-        <v>0.6936598420143127</v>
+        <v>103.7515869140625</v>
       </c>
       <c r="H90">
-        <v>1.031503915786743</v>
+        <v>0.1087311059236526</v>
       </c>
       <c r="I90">
-        <v>75975.59375</v>
+        <v>0.0009995077271014452</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3034,13 +3034,13 @@
         <v>74177.05785785212</v>
       </c>
       <c r="G91">
-        <v>0.7143449187278748</v>
+        <v>97.08790588378906</v>
       </c>
       <c r="H91">
-        <v>1.032370328903198</v>
+        <v>0.1037214025855064</v>
       </c>
       <c r="I91">
-        <v>74252.875</v>
+        <v>0.00106118293479085</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3063,13 +3063,13 @@
         <v>84349.1162867714</v>
       </c>
       <c r="G92">
-        <v>0.7220648527145386</v>
+        <v>93.01198577880859</v>
       </c>
       <c r="H92">
-        <v>1.034156084060669</v>
+        <v>0.09593512862920761</v>
       </c>
       <c r="I92">
-        <v>84377.7734375</v>
+        <v>0.0009494195692241192</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -3092,13 +3092,13 @@
         <v>90936.71391413134</v>
       </c>
       <c r="G93">
-        <v>0.7084622979164124</v>
+        <v>97.29978179931641</v>
       </c>
       <c r="H93">
-        <v>1.033885598182678</v>
+        <v>0.0950256735086441</v>
       </c>
       <c r="I93">
-        <v>90434.3203125</v>
+        <v>0.0008556626853533089</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -3121,13 +3121,13 @@
         <v>75602.5895983599</v>
       </c>
       <c r="G94">
-        <v>0.7574493885040283</v>
+        <v>74.5960693359375</v>
       </c>
       <c r="H94">
-        <v>1.036322593688965</v>
+        <v>0.09427420794963837</v>
       </c>
       <c r="I94">
-        <v>75960.4375</v>
+        <v>0.001129039446823299</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3150,13 +3150,13 @@
         <v>81350.10967911783</v>
       </c>
       <c r="G95">
-        <v>0.6619002223014832</v>
+        <v>129.4559936523438</v>
       </c>
       <c r="H95">
-        <v>1.030957341194153</v>
+        <v>0.1016243770718575</v>
       </c>
       <c r="I95">
-        <v>81528.109375</v>
+        <v>0.0008820169023238122</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3179,13 +3179,13 @@
         <v>77350.32360771715</v>
       </c>
       <c r="G96">
-        <v>0.7055090069770813</v>
+        <v>97.19788360595703</v>
       </c>
       <c r="H96">
-        <v>1.032380938529968</v>
+        <v>0.1059783771634102</v>
       </c>
       <c r="I96">
-        <v>77338.6171875</v>
+        <v>0.001003028824925423</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3208,13 +3208,13 @@
         <v>88999.55306112269</v>
       </c>
       <c r="G97">
-        <v>0.7152878046035767</v>
+        <v>87.52497863769531</v>
       </c>
       <c r="H97">
-        <v>1.034407615661621</v>
+        <v>0.09931990504264832</v>
       </c>
       <c r="I97">
-        <v>88633.7265625</v>
+        <v>0.0008953398792073131</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3237,13 +3237,13 @@
         <v>92767.28100028589</v>
       </c>
       <c r="G98">
-        <v>0.7089437246322632</v>
+        <v>98.22142028808594</v>
       </c>
       <c r="H98">
-        <v>1.034107804298401</v>
+        <v>0.09311936795711517</v>
       </c>
       <c r="I98">
-        <v>91985.09375</v>
+        <v>0.0008378461934626102</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3266,13 +3266,13 @@
         <v>74613.77525697168</v>
       </c>
       <c r="G99">
-        <v>0.7571243643760681</v>
+        <v>64.81377410888672</v>
       </c>
       <c r="H99">
-        <v>1.036565542221069</v>
+        <v>0.1001377329230309</v>
       </c>
       <c r="I99">
-        <v>75176.25</v>
+        <v>0.001141287735663354</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3295,13 +3295,13 @@
         <v>69935.752314963</v>
       </c>
       <c r="G100">
-        <v>0.7485681176185608</v>
+        <v>110.8403244018555</v>
       </c>
       <c r="H100">
-        <v>1.033669352531433</v>
+        <v>0.08295104652643204</v>
       </c>
       <c r="I100">
-        <v>70412.1015625</v>
+        <v>0.001170862815342844</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3324,13 +3324,13 @@
         <v>70817.75348355506</v>
       </c>
       <c r="G101">
-        <v>0.7481361031532288</v>
+        <v>68.18665313720703</v>
       </c>
       <c r="H101">
-        <v>1.035487771034241</v>
+        <v>0.1057525128126144</v>
       </c>
       <c r="I101">
-        <v>71437.8984375</v>
+        <v>0.001170065603218973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Layouts and Styles
</commit_message>
<xml_diff>
--- a/datasets/MLP_Validation_Dataset.xlsx
+++ b/datasets/MLP_Validation_Dataset.xlsx
@@ -435,2902 +435,2902 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>80.47950312370034</v>
+        <v>124.3933299532707</v>
       </c>
       <c r="B2">
-        <v>0.09239295734468765</v>
+        <v>0.09407557004821653</v>
       </c>
       <c r="C2">
-        <v>0.0007239956811404301</v>
+        <v>0.0008862284955878868</v>
       </c>
       <c r="D2">
-        <v>0.7148542594299597</v>
+        <v>0.6784197946431981</v>
       </c>
       <c r="E2">
-        <v>1.037657893482221</v>
+        <v>1.032521051561644</v>
       </c>
       <c r="F2">
-        <v>110714.6618363113</v>
+        <v>83409.2684077368</v>
       </c>
       <c r="G2">
-        <v>79.75212097167969</v>
+        <v>118.9669570922852</v>
       </c>
       <c r="H2">
-        <v>0.09297946840524673</v>
+        <v>0.09846629202365875</v>
       </c>
       <c r="I2">
-        <v>0.0007230084738694131</v>
+        <v>0.000886996858753264</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>89.67928005448476</v>
+        <v>116.4428399619183</v>
       </c>
       <c r="B3">
-        <v>0.08337182908089882</v>
+        <v>0.1257574850381628</v>
       </c>
       <c r="C3">
-        <v>0.001083823063645076</v>
+        <v>0.0009238209183284484</v>
       </c>
       <c r="D3">
-        <v>0.7616355600549359</v>
+        <v>0.6416620503710493</v>
       </c>
       <c r="E3">
-        <v>1.037050513453626</v>
+        <v>1.030509950366821</v>
       </c>
       <c r="F3">
-        <v>78814.76879823163</v>
+        <v>75107.54906879865</v>
       </c>
       <c r="G3">
-        <v>89.54709625244141</v>
+        <v>117.2525253295898</v>
       </c>
       <c r="H3">
-        <v>0.08366125822067261</v>
+        <v>0.1245705112814903</v>
       </c>
       <c r="I3">
-        <v>0.001081483671441674</v>
+        <v>0.0009223023080267012</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <v>110.8209199609001</v>
+        <v>89.9887091217185</v>
       </c>
       <c r="B4">
-        <v>0.07483192020831066</v>
+        <v>0.07597689581327628</v>
       </c>
       <c r="C4">
-        <v>0.0009449817450038469</v>
+        <v>0.001014982265352558</v>
       </c>
       <c r="D4">
-        <v>0.745030186083138</v>
+        <v>0.7718979960987465</v>
       </c>
       <c r="E4">
-        <v>1.035866141498359</v>
+        <v>1.039101555760223</v>
       </c>
       <c r="F4">
-        <v>87584.8689481738</v>
+        <v>85842.17804485078</v>
       </c>
       <c r="G4">
-        <v>111.4523086547852</v>
+        <v>90.45449829101562</v>
       </c>
       <c r="H4">
-        <v>0.07496283948421478</v>
+        <v>0.0756971687078476</v>
       </c>
       <c r="I4">
-        <v>0.0009426595643162727</v>
+        <v>0.001012900262139738</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
-        <v>73.79245710031783</v>
+        <v>74.8660833992798</v>
       </c>
       <c r="B5">
-        <v>0.0751186553871222</v>
+        <v>0.1267180920087448</v>
       </c>
       <c r="C5">
-        <v>0.0009264439435533324</v>
+        <v>0.001150357013757392</v>
       </c>
       <c r="D5">
-        <v>0.78228369652713</v>
+        <v>0.7032906533559896</v>
       </c>
       <c r="E5">
-        <v>1.045092820041995</v>
+        <v>1.03292318239526</v>
       </c>
       <c r="F5">
-        <v>97240.64886250457</v>
+        <v>67653.33328088738</v>
       </c>
       <c r="G5">
-        <v>69.42737579345703</v>
+        <v>75.66586303710938</v>
       </c>
       <c r="H5">
-        <v>0.0768093541264534</v>
+        <v>0.1248805001378059</v>
       </c>
       <c r="I5">
-        <v>0.0009390211198478937</v>
+        <v>0.001151624135673046</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6">
-        <v>106.4349624406925</v>
+        <v>94.43447028482844</v>
       </c>
       <c r="B6">
-        <v>0.08328378677756634</v>
+        <v>0.1221693118327979</v>
       </c>
       <c r="C6">
-        <v>0.001185618982893519</v>
+        <v>0.0009001044794747651</v>
       </c>
       <c r="D6">
-        <v>0.7549607388106844</v>
+        <v>0.6709896671507818</v>
       </c>
       <c r="E6">
-        <v>1.034312784197991</v>
+        <v>1.031087046424282</v>
       </c>
       <c r="F6">
-        <v>70553.25308145517</v>
+        <v>81501.43078807385</v>
       </c>
       <c r="G6">
-        <v>113.9127807617188</v>
+        <v>92.75955963134766</v>
       </c>
       <c r="H6">
-        <v>0.08137539774179459</v>
+        <v>0.1228116229176521</v>
       </c>
       <c r="I6">
-        <v>0.001188633963465691</v>
+        <v>0.0008978932164609432</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7">
-        <v>98.65879017258494</v>
+        <v>83.93404853025656</v>
       </c>
       <c r="B7">
-        <v>0.07600084365529332</v>
+        <v>0.09724974381445312</v>
       </c>
       <c r="C7">
-        <v>0.001125421276109974</v>
+        <v>0.001254495259972458</v>
       </c>
       <c r="D7">
-        <v>0.7726512369998835</v>
+        <v>0.748545709022876</v>
       </c>
       <c r="E7">
-        <v>1.037115564928178</v>
+        <v>1.035210057907326</v>
       </c>
       <c r="F7">
-        <v>76929.05447955293</v>
+        <v>66574.34531374181</v>
       </c>
       <c r="G7">
-        <v>99.45830535888672</v>
+        <v>84.42269134521484</v>
       </c>
       <c r="H7">
-        <v>0.07635018974542618</v>
+        <v>0.09730326384305954</v>
       </c>
       <c r="I7">
-        <v>0.001123866415582597</v>
+        <v>0.00125624961219728</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
-        <v>87.03999860572607</v>
+        <v>77.94925808547897</v>
       </c>
       <c r="B8">
-        <v>0.08590238190186891</v>
+        <v>0.0896020529060956</v>
       </c>
       <c r="C8">
-        <v>0.001272600289235615</v>
+        <v>0.001217391128101541</v>
       </c>
       <c r="D8">
-        <v>0.7686426747971807</v>
+        <v>0.7648503164060173</v>
       </c>
       <c r="E8">
-        <v>1.036880237584814</v>
+        <v>1.03844357978956</v>
       </c>
       <c r="F8">
-        <v>67775.15318781788</v>
+        <v>70911.24322022406</v>
       </c>
       <c r="G8">
-        <v>86.98581695556641</v>
+        <v>79.07155609130859</v>
       </c>
       <c r="H8">
-        <v>0.0866340696811676</v>
+        <v>0.08825353533029556</v>
       </c>
       <c r="I8">
-        <v>0.001269801403395832</v>
+        <v>0.001214876538142562</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
-        <v>84.30479685544348</v>
+        <v>73.20563090720951</v>
       </c>
       <c r="B9">
-        <v>0.07396896772701729</v>
+        <v>0.08396464775674342</v>
       </c>
       <c r="C9">
-        <v>0.0009111617442974144</v>
+        <v>0.0007292141775853172</v>
       </c>
       <c r="D9">
-        <v>0.7728103531743354</v>
+        <v>0.7433984222429161</v>
       </c>
       <c r="E9">
-        <v>1.041503063754441</v>
+        <v>1.042329384738902</v>
       </c>
       <c r="F9">
-        <v>96481.13007662418</v>
+        <v>116173.4030148928</v>
       </c>
       <c r="G9">
-        <v>82.75128173828125</v>
+        <v>73.19467163085938</v>
       </c>
       <c r="H9">
-        <v>0.07491426169872284</v>
+        <v>0.08252929896116257</v>
       </c>
       <c r="I9">
-        <v>0.0009137484012171626</v>
+        <v>0.0007127003045752645</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10">
-        <v>100.8707645979254</v>
+        <v>113.5356618526347</v>
       </c>
       <c r="B10">
-        <v>0.07393629203259555</v>
+        <v>0.1068678823886125</v>
       </c>
       <c r="C10">
-        <v>0.001238525658789643</v>
+        <v>0.0008521855145540937</v>
       </c>
       <c r="D10">
-        <v>0.7828476779742215</v>
+        <v>0.6633218866632808</v>
       </c>
       <c r="E10">
-        <v>1.037145661916517</v>
+        <v>1.031685865077828</v>
       </c>
       <c r="F10">
-        <v>70858.65038252129</v>
+        <v>84746.04781257008</v>
       </c>
       <c r="G10">
-        <v>101.3134689331055</v>
+        <v>114.9007949829102</v>
       </c>
       <c r="H10">
-        <v>0.07427240908145905</v>
+        <v>0.1058211252093315</v>
       </c>
       <c r="I10">
-        <v>0.001237468677572906</v>
+        <v>0.0008518047397956252</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11">
-        <v>92.07565483222247</v>
+        <v>70.68564751750186</v>
       </c>
       <c r="B11">
-        <v>0.1213765707773669</v>
+        <v>0.07198447548853035</v>
       </c>
       <c r="C11">
-        <v>0.001161980311750053</v>
+        <v>0.0009676813075955211</v>
       </c>
       <c r="D11">
-        <v>0.6986465246035998</v>
+        <v>0.794812134313133</v>
       </c>
       <c r="E11">
-        <v>1.030967409724419</v>
+        <v>1.048020977844326</v>
       </c>
       <c r="F11">
-        <v>65882.93905127795</v>
+        <v>95481.35117599939</v>
       </c>
       <c r="G11">
-        <v>106.1813507080078</v>
+        <v>64.12001037597656</v>
       </c>
       <c r="H11">
-        <v>0.1133106648921967</v>
+        <v>0.07391037046909332</v>
       </c>
       <c r="I11">
-        <v>0.001160298474133015</v>
+        <v>0.0009916506242007017</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12">
-        <v>97.39119347575932</v>
+        <v>116.2348449101666</v>
       </c>
       <c r="B12">
-        <v>0.07972721564253001</v>
+        <v>0.0709363638668097</v>
       </c>
       <c r="C12">
-        <v>0.0009144547909568278</v>
+        <v>0.0007627767332454845</v>
       </c>
       <c r="D12">
-        <v>0.7456258922776794</v>
+        <v>0.7160050307302082</v>
       </c>
       <c r="E12">
-        <v>1.036677984385607</v>
+        <v>1.036415571198188</v>
       </c>
       <c r="F12">
-        <v>91078.41849770934</v>
+        <v>104049.0177463293</v>
       </c>
       <c r="G12">
-        <v>98.46724700927734</v>
+        <v>101.2191314697266</v>
       </c>
       <c r="H12">
-        <v>0.07945484668016434</v>
+        <v>0.08048275113105774</v>
       </c>
       <c r="I12">
-        <v>0.0009120404720306396</v>
+        <v>0.0007677354151383042</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13">
-        <v>90.2486429058544</v>
+        <v>78.8167987240225</v>
       </c>
       <c r="B13">
-        <v>0.1035809443494069</v>
+        <v>0.09572774334989427</v>
       </c>
       <c r="C13">
-        <v>0.001072999261871955</v>
+        <v>0.0009090855934200982</v>
       </c>
       <c r="D13">
-        <v>0.7224579881240755</v>
+        <v>0.7341306222439513</v>
       </c>
       <c r="E13">
-        <v>1.033217153180326</v>
+        <v>1.037064631932724</v>
       </c>
       <c r="F13">
-        <v>74453.07845140826</v>
+        <v>90574.8247297559</v>
       </c>
       <c r="G13">
-        <v>101.1958465576172</v>
+        <v>78.97686004638672</v>
       </c>
       <c r="H13">
-        <v>0.09819482266902924</v>
+        <v>0.09638064354658127</v>
       </c>
       <c r="I13">
-        <v>0.001074345083907247</v>
+        <v>0.0009047820931300521</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14">
-        <v>128.2296216157586</v>
+        <v>74.77132495520534</v>
       </c>
       <c r="B14">
-        <v>0.1164073326669418</v>
+        <v>0.07408444443848322</v>
       </c>
       <c r="C14">
-        <v>0.0008731419745910173</v>
+        <v>0.001144058515370609</v>
       </c>
       <c r="D14">
-        <v>0.6320502746174453</v>
+        <v>0.7956725026218914</v>
       </c>
       <c r="E14">
-        <v>1.031517906237351</v>
+        <v>1.044819059822599</v>
       </c>
       <c r="F14">
-        <v>78135.11268005935</v>
+        <v>80121.79010712411</v>
       </c>
       <c r="G14">
-        <v>127.3419342041016</v>
+        <v>72.65552520751953</v>
       </c>
       <c r="H14">
-        <v>0.1170404180884361</v>
+        <v>0.0746302604675293</v>
       </c>
       <c r="I14">
-        <v>0.0008698375895619392</v>
+        <v>0.001160135725513101</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15">
-        <v>78.00636590473624</v>
+        <v>75.37618205431632</v>
       </c>
       <c r="B15">
-        <v>0.097384573920344</v>
+        <v>0.08511645929476558</v>
       </c>
       <c r="C15">
-        <v>0.001224639950244905</v>
+        <v>0.001108308688685695</v>
       </c>
       <c r="D15">
-        <v>0.7507819662196481</v>
+        <v>0.7707258071110492</v>
       </c>
       <c r="E15">
-        <v>1.036648787614249</v>
+        <v>1.040615406203984</v>
       </c>
       <c r="F15">
-        <v>68769.88104121231</v>
+        <v>79038.84303120871</v>
       </c>
       <c r="G15">
-        <v>77.52542114257812</v>
+        <v>76.23108673095703</v>
       </c>
       <c r="H15">
-        <v>0.09769745171070099</v>
+        <v>0.08453262597322464</v>
       </c>
       <c r="I15">
-        <v>0.001223880564793944</v>
+        <v>0.001108782133087516</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16">
-        <v>75.80823719070246</v>
+        <v>110.3228684412349</v>
       </c>
       <c r="B16">
-        <v>0.07920213267156075</v>
+        <v>0.08326965492076503</v>
       </c>
       <c r="C16">
-        <v>0.0007674563903273868</v>
+        <v>0.001073430657139603</v>
       </c>
       <c r="D16">
-        <v>0.7551169660496789</v>
+        <v>0.7418184427016393</v>
       </c>
       <c r="E16">
-        <v>1.042849564994777</v>
+        <v>1.034069663720008</v>
       </c>
       <c r="F16">
-        <v>112338.4518110541</v>
+        <v>76365.10801542967</v>
       </c>
       <c r="G16">
-        <v>75.03432464599609</v>
+        <v>118.7014846801758</v>
       </c>
       <c r="H16">
-        <v>0.07915347814559937</v>
+        <v>0.07900670170783997</v>
       </c>
       <c r="I16">
-        <v>0.0007577281212434173</v>
+        <v>0.001072810729965568</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17">
-        <v>90.60350372745496</v>
+        <v>84.72203259117069</v>
       </c>
       <c r="B17">
-        <v>0.08197576852720687</v>
+        <v>0.08519147162337112</v>
       </c>
       <c r="C17">
-        <v>0.0008274606167764246</v>
+        <v>0.001126317041633407</v>
       </c>
       <c r="D17">
-        <v>0.737666059193431</v>
+        <v>0.764648901271565</v>
       </c>
       <c r="E17">
-        <v>1.037557826832974</v>
+        <v>1.03771950408901</v>
       </c>
       <c r="F17">
-        <v>99907.35472228569</v>
+        <v>76377.44331391205</v>
       </c>
       <c r="G17">
-        <v>90.96507263183594</v>
+        <v>85.87974548339844</v>
       </c>
       <c r="H17">
-        <v>0.08217146247625351</v>
+        <v>0.08418426662683487</v>
       </c>
       <c r="I17">
-        <v>0.0008223837940022349</v>
+        <v>0.001122905407100916</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18">
-        <v>105.4616140522295</v>
+        <v>95.23236800080591</v>
       </c>
       <c r="B18">
-        <v>0.09597905237687085</v>
+        <v>0.07786331387291547</v>
       </c>
       <c r="C18">
-        <v>0.0008098199752479526</v>
+        <v>0.0008229542121758211</v>
       </c>
       <c r="D18">
-        <v>0.6863786183384455</v>
+        <v>0.7399345090497457</v>
       </c>
       <c r="E18">
-        <v>1.03309890771149</v>
+        <v>1.037668255044031</v>
       </c>
       <c r="F18">
-        <v>93081.67690294122</v>
+        <v>100708.8082984162</v>
       </c>
       <c r="G18">
-        <v>93.49736022949219</v>
+        <v>96.33669281005859</v>
       </c>
       <c r="H18">
-        <v>0.1059889942407608</v>
+        <v>0.07730789482593536</v>
       </c>
       <c r="I18">
-        <v>0.0008154105744324625</v>
+        <v>0.0008200373849831522</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19">
-        <v>109.5505883110017</v>
+        <v>103.442127479435</v>
       </c>
       <c r="B19">
-        <v>0.1016940453507122</v>
+        <v>0.07072217337385926</v>
       </c>
       <c r="C19">
-        <v>0.0009418156014425732</v>
+        <v>0.0009050188689188393</v>
       </c>
       <c r="D19">
-        <v>0.6915085550610071</v>
+        <v>0.7580328990929878</v>
       </c>
       <c r="E19">
-        <v>1.031925803288023</v>
+        <v>1.038020268327935</v>
       </c>
       <c r="F19">
-        <v>80308.98160370781</v>
+        <v>93872.56742397539</v>
       </c>
       <c r="G19">
-        <v>99.27290344238281</v>
+        <v>101.7036209106445</v>
       </c>
       <c r="H19">
-        <v>0.1087920889258385</v>
+        <v>0.07165741175413132</v>
       </c>
       <c r="I19">
-        <v>0.000945953419432044</v>
+        <v>0.000905612192582339</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20">
-        <v>93.83540483008252</v>
+        <v>121.6330704297276</v>
       </c>
       <c r="B20">
-        <v>0.0909664175229121</v>
+        <v>0.07692905782832489</v>
       </c>
       <c r="C20">
-        <v>0.001147139776019277</v>
+        <v>0.001105745489366478</v>
       </c>
       <c r="D20">
-        <v>0.74740111122718</v>
+        <v>0.7479044580181887</v>
       </c>
       <c r="E20">
-        <v>1.034610430079018</v>
+        <v>1.03425770292703</v>
       </c>
       <c r="F20">
-        <v>72418.37381022613</v>
+        <v>74609.31339163485</v>
       </c>
       <c r="G20">
-        <v>93.18444061279297</v>
+        <v>118.4432144165039</v>
       </c>
       <c r="H20">
-        <v>0.09092806279659271</v>
+        <v>0.07802055031061172</v>
       </c>
       <c r="I20">
-        <v>0.001150672673247755</v>
+        <v>0.001109752687625587</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21">
-        <v>129.9566796353303</v>
+        <v>113.6226557626797</v>
       </c>
       <c r="B21">
-        <v>0.1168887760140797</v>
+        <v>0.1071088155707649</v>
       </c>
       <c r="C21">
-        <v>0.001016144469431308</v>
+        <v>0.001227540857818796</v>
       </c>
       <c r="D21">
-        <v>0.6528624185802553</v>
+        <v>0.7077726126953642</v>
       </c>
       <c r="E21">
-        <v>1.031010373892499</v>
+        <v>1.030868173553104</v>
       </c>
       <c r="F21">
-        <v>69354.92481327662</v>
+        <v>62856.18187144435</v>
       </c>
       <c r="G21">
-        <v>129.8472595214844</v>
+        <v>107.9959487915039</v>
       </c>
       <c r="H21">
-        <v>0.1171072944998741</v>
+        <v>0.1102267950773239</v>
       </c>
       <c r="I21">
-        <v>0.001018858747556806</v>
+        <v>0.001231402158737183</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22">
-        <v>91.11357977158256</v>
+        <v>86.21967431432287</v>
       </c>
       <c r="B22">
-        <v>0.1150612989313839</v>
+        <v>0.128455372769083</v>
       </c>
       <c r="C22">
-        <v>0.0009926057941229245</v>
+        <v>0.001026206832296857</v>
       </c>
       <c r="D22">
-        <v>0.6959553476844512</v>
+        <v>0.6839160097762933</v>
       </c>
       <c r="E22">
-        <v>1.031848404782693</v>
+        <v>1.031080013828039</v>
       </c>
       <c r="F22">
-        <v>77046.07244606676</v>
+        <v>73078.70595254088</v>
       </c>
       <c r="G22">
-        <v>103.6271133422852</v>
+        <v>104.6735153198242</v>
       </c>
       <c r="H22">
-        <v>0.1062049195170403</v>
+        <v>0.1153660863637924</v>
       </c>
       <c r="I22">
-        <v>0.0009920671582221985</v>
+        <v>0.001021843170747161</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23">
-        <v>113.2844000775972</v>
+        <v>77.88896795746766</v>
       </c>
       <c r="B23">
-        <v>0.1256327084423871</v>
+        <v>0.1294207000936536</v>
       </c>
       <c r="C23">
-        <v>0.0007003275789381973</v>
+        <v>0.000869619790567322</v>
       </c>
       <c r="D23">
-        <v>0.6014607693384898</v>
+        <v>0.6771432974829313</v>
       </c>
       <c r="E23">
-        <v>1.031412505497343</v>
+        <v>1.032325862517038</v>
       </c>
       <c r="F23">
-        <v>92838.36523798428</v>
+        <v>85823.20635196286</v>
       </c>
       <c r="G23">
-        <v>112.4546508789062</v>
+        <v>107.4036331176758</v>
       </c>
       <c r="H23">
-        <v>0.1266688257455826</v>
+        <v>0.1059320792555809</v>
       </c>
       <c r="I23">
-        <v>0.0006963207270018756</v>
+        <v>0.0008659764425829053</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24">
-        <v>108.2549616718476</v>
+        <v>73.32245922527187</v>
       </c>
       <c r="B24">
-        <v>0.07173715294161764</v>
+        <v>0.09454324572238371</v>
       </c>
       <c r="C24">
-        <v>0.0009552410352130327</v>
+        <v>0.0007181411548035895</v>
       </c>
       <c r="D24">
-        <v>0.7565650575592371</v>
+        <v>0.7206966223399396</v>
       </c>
       <c r="E24">
-        <v>1.036924640141883</v>
+        <v>1.039301501758527</v>
       </c>
       <c r="F24">
-        <v>88386.57695820175</v>
+        <v>113238.0637018745</v>
       </c>
       <c r="G24">
-        <v>107.526252746582</v>
+        <v>72.77150726318359</v>
       </c>
       <c r="H24">
-        <v>0.07269988209009171</v>
+        <v>0.09486087411642075</v>
       </c>
       <c r="I24">
-        <v>0.000960936420597136</v>
+        <v>0.0007132915197871625</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25">
-        <v>118.7832317948476</v>
+        <v>88.09591806885655</v>
       </c>
       <c r="B25">
-        <v>0.1237414774726122</v>
+        <v>0.07977726556279632</v>
       </c>
       <c r="C25">
-        <v>0.000738132264901695</v>
+        <v>0.001126202097384528</v>
       </c>
       <c r="D25">
-        <v>0.6051214927972042</v>
+        <v>0.7731445724155795</v>
       </c>
       <c r="E25">
-        <v>1.031522256378468</v>
+        <v>1.038318564867881</v>
       </c>
       <c r="F25">
-        <v>88510.38069130151</v>
+        <v>77362.88486886748</v>
       </c>
       <c r="G25">
-        <v>118.0151290893555</v>
+        <v>89.11637878417969</v>
       </c>
       <c r="H25">
-        <v>0.1246507912874222</v>
+        <v>0.07897152006626129</v>
       </c>
       <c r="I25">
-        <v>0.0007369038066826761</v>
+        <v>0.001122327172197402</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26">
-        <v>128.5735398072292</v>
+        <v>85.72708895438069</v>
       </c>
       <c r="B26">
-        <v>0.09355412730772907</v>
+        <v>0.1083257054419918</v>
       </c>
       <c r="C26">
-        <v>0.0008249519512728903</v>
+        <v>0.0007047304621050643</v>
       </c>
       <c r="D26">
-        <v>0.6619779054087238</v>
+        <v>0.674312012594977</v>
       </c>
       <c r="E26">
-        <v>1.032779265983835</v>
+        <v>1.033763432400564</v>
       </c>
       <c r="F26">
-        <v>87259.22312703876</v>
+        <v>105728.7991686211</v>
       </c>
       <c r="G26">
-        <v>128.1912384033203</v>
+        <v>87.72163391113281</v>
       </c>
       <c r="H26">
-        <v>0.09278549253940582</v>
+        <v>0.1063713729381561</v>
       </c>
       <c r="I26">
-        <v>0.0008264060015790164</v>
+        <v>0.0006962359184399247</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27">
-        <v>123.3876193867324</v>
+        <v>97.36843400802877</v>
       </c>
       <c r="B27">
-        <v>0.1227023497227996</v>
+        <v>0.09941832079292423</v>
       </c>
       <c r="C27">
-        <v>0.001259436363376297</v>
+        <v>0.0009236074418925973</v>
       </c>
       <c r="D27">
-        <v>0.6774113521556409</v>
+        <v>0.7077344103635644</v>
       </c>
       <c r="E27">
-        <v>1.029975939243343</v>
+        <v>1.033136866007716</v>
       </c>
       <c r="F27">
-        <v>58129.14017715984</v>
+        <v>84477.40470257214</v>
       </c>
       <c r="G27">
-        <v>122.3028869628906</v>
+        <v>102.1720504760742</v>
       </c>
       <c r="H27">
-        <v>0.1233147084712982</v>
+        <v>0.09669432044029236</v>
       </c>
       <c r="I27">
-        <v>0.001257339841686189</v>
+        <v>0.0009203733643516898</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28">
-        <v>115.8737184614625</v>
+        <v>110.9968801328608</v>
       </c>
       <c r="B28">
-        <v>0.1114470865693918</v>
+        <v>0.1293645866370659</v>
       </c>
       <c r="C28">
-        <v>0.0008292389226059429</v>
+        <v>0.001018322328737669</v>
       </c>
       <c r="D28">
-        <v>0.6482159643812835</v>
+        <v>0.6557880806920737</v>
       </c>
       <c r="E28">
-        <v>1.031484946473459</v>
+        <v>1.029983751965406</v>
       </c>
       <c r="F28">
-        <v>84867.05205977788</v>
+        <v>69737.0007968694</v>
       </c>
       <c r="G28">
-        <v>116.1699981689453</v>
+        <v>111.9937744140625</v>
       </c>
       <c r="H28">
-        <v>0.1113805547356606</v>
+        <v>0.1280508190393448</v>
       </c>
       <c r="I28">
-        <v>0.0008288726094178855</v>
+        <v>0.001025634584948421</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29">
-        <v>111.8949086690974</v>
+        <v>111.7375267383315</v>
       </c>
       <c r="B29">
-        <v>0.1292409254244381</v>
+        <v>0.07391825242910682</v>
       </c>
       <c r="C29">
-        <v>0.001215002583180557</v>
+        <v>0.001253266877060316</v>
       </c>
       <c r="D29">
-        <v>0.674255463494057</v>
+        <v>0.7757659767250484</v>
       </c>
       <c r="E29">
-        <v>1.029631416784115</v>
+        <v>1.035563829912116</v>
       </c>
       <c r="F29">
-        <v>60101.35602195264</v>
+        <v>68866.08159224331</v>
       </c>
       <c r="G29">
-        <v>110.3302001953125</v>
+        <v>111.5711898803711</v>
       </c>
       <c r="H29">
-        <v>0.1301198303699493</v>
+        <v>0.07335401326417923</v>
       </c>
       <c r="I29">
-        <v>0.001208516885526478</v>
+        <v>0.001251352136023343</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30">
-        <v>90.12989018055399</v>
+        <v>87.01113079493</v>
       </c>
       <c r="B30">
-        <v>0.1155569471030001</v>
+        <v>0.1169940662988288</v>
       </c>
       <c r="C30">
-        <v>0.001181736022936801</v>
+        <v>0.0007536967270197401</v>
       </c>
       <c r="D30">
-        <v>0.7102333799737831</v>
+        <v>0.6672539329429855</v>
       </c>
       <c r="E30">
-        <v>1.031703854837487</v>
+        <v>1.032548388441922</v>
       </c>
       <c r="F30">
-        <v>66091.3562768952</v>
+        <v>97368.78087714546</v>
       </c>
       <c r="G30">
-        <v>111.0831069946289</v>
+        <v>88.40513610839844</v>
       </c>
       <c r="H30">
-        <v>0.104269728064537</v>
+        <v>0.114439956843853</v>
       </c>
       <c r="I30">
-        <v>0.001179161132313311</v>
+        <v>0.0007519418140873313</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31">
-        <v>78.86113469240244</v>
+        <v>92.79561735400723</v>
       </c>
       <c r="B31">
-        <v>0.0918726775598072</v>
+        <v>0.08730390983988964</v>
       </c>
       <c r="C31">
-        <v>0.0007954877421653457</v>
+        <v>0.0009435653931809701</v>
       </c>
       <c r="D31">
-        <v>0.7287884903981767</v>
+        <v>0.7383504988680027</v>
       </c>
       <c r="E31">
-        <v>1.038094802825155</v>
+        <v>1.035754346555935</v>
       </c>
       <c r="F31">
-        <v>102999.9399945368</v>
+        <v>87220.0883744399</v>
       </c>
       <c r="G31">
-        <v>78.43529510498047</v>
+        <v>93.76967620849609</v>
       </c>
       <c r="H31">
-        <v>0.09235022217035294</v>
+        <v>0.08689599484205246</v>
       </c>
       <c r="I31">
-        <v>0.0007984889089129865</v>
+        <v>0.0009384458535350859</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32">
-        <v>73.75816018358859</v>
+        <v>80.86905770421419</v>
       </c>
       <c r="B32">
-        <v>0.1000637903700851</v>
+        <v>0.08448511720459445</v>
       </c>
       <c r="C32">
-        <v>0.001063427174362167</v>
+        <v>0.0007145879198260947</v>
       </c>
       <c r="D32">
-        <v>0.7419344320137233</v>
+        <v>0.7285468765524257</v>
       </c>
       <c r="E32">
-        <v>1.037425163918059</v>
+        <v>1.039504992586646</v>
       </c>
       <c r="F32">
-        <v>78446.7561659481</v>
+        <v>115014.1679102822</v>
       </c>
       <c r="G32">
-        <v>73.11083221435547</v>
+        <v>81.06871795654297</v>
       </c>
       <c r="H32">
-        <v>0.1009776294231415</v>
+        <v>0.08405093103647232</v>
       </c>
       <c r="I32">
-        <v>0.001059458707459271</v>
+        <v>0.0007065714453347027</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33">
-        <v>84.51410225208909</v>
+        <v>117.3127307383911</v>
       </c>
       <c r="B33">
-        <v>0.09258334931166108</v>
+        <v>0.1097502742919606</v>
       </c>
       <c r="C33">
-        <v>0.0007693971231430079</v>
+        <v>0.0009055665906049541</v>
       </c>
       <c r="D33">
-        <v>0.7158396833095715</v>
+        <v>0.6626127322955803</v>
       </c>
       <c r="E33">
-        <v>1.036550635565334</v>
+        <v>1.031327446078763</v>
       </c>
       <c r="F33">
-        <v>103940.0373470859</v>
+        <v>79478.93779205675</v>
       </c>
       <c r="G33">
-        <v>97.99827575683594</v>
+        <v>118.0692138671875</v>
       </c>
       <c r="H33">
-        <v>0.08354198932647705</v>
+        <v>0.1088730245828629</v>
       </c>
       <c r="I33">
-        <v>0.0007745617185719311</v>
+        <v>0.0008994752424769104</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34">
-        <v>95.93688887087791</v>
+        <v>73.41088458599442</v>
       </c>
       <c r="B34">
-        <v>0.09189471016127429</v>
+        <v>0.08476379109945789</v>
       </c>
       <c r="C34">
-        <v>0.001136732895021707</v>
+        <v>0.001073338635303877</v>
       </c>
       <c r="D34">
-        <v>0.74317886691169</v>
+        <v>0.7712150790207645</v>
       </c>
       <c r="E34">
-        <v>1.034125868657118</v>
+        <v>1.04153184931658</v>
       </c>
       <c r="F34">
-        <v>72512.80722001196</v>
+        <v>81894.96184519191</v>
       </c>
       <c r="G34">
-        <v>95.67485809326172</v>
+        <v>73.48490905761719</v>
       </c>
       <c r="H34">
-        <v>0.09278919547796249</v>
+        <v>0.08452140539884567</v>
       </c>
       <c r="I34">
-        <v>0.001142073539085686</v>
+        <v>0.001078406232409179</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35">
-        <v>101.3197764177989</v>
+        <v>111.8198345034992</v>
       </c>
       <c r="B35">
-        <v>0.0856542699628636</v>
+        <v>0.1099515470535513</v>
       </c>
       <c r="C35">
-        <v>0.001082477366423324</v>
+        <v>0.000867440768937159</v>
       </c>
       <c r="D35">
-        <v>0.7463949669992432</v>
+        <v>0.6630529015050783</v>
       </c>
       <c r="E35">
-        <v>1.034605699648733</v>
+        <v>1.031441086289076</v>
       </c>
       <c r="F35">
-        <v>76504.91466527247</v>
+        <v>83198.63610148398</v>
       </c>
       <c r="G35">
-        <v>114.9620819091797</v>
+        <v>111.854118347168</v>
       </c>
       <c r="H35">
-        <v>0.07929599285125732</v>
+        <v>0.1101681888103485</v>
       </c>
       <c r="I35">
-        <v>0.001075986190699041</v>
+        <v>0.0008640999440103769</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36">
-        <v>116.3850132432923</v>
+        <v>116.7217237564662</v>
       </c>
       <c r="B36">
-        <v>0.0997582177224082</v>
+        <v>0.1010385110321373</v>
       </c>
       <c r="C36">
-        <v>0.001187163137014612</v>
+        <v>0.0008258499697933812</v>
       </c>
       <c r="D36">
-        <v>0.7147880752932645</v>
+        <v>0.6643437527588949</v>
       </c>
       <c r="E36">
-        <v>1.031475902851138</v>
+        <v>1.032186963588209</v>
       </c>
       <c r="F36">
-        <v>65754.04768377355</v>
+        <v>87641.68174692536</v>
       </c>
       <c r="G36">
-        <v>107.1488876342773</v>
+        <v>118.5785827636719</v>
       </c>
       <c r="H36">
-        <v>0.1050450280308723</v>
+        <v>0.09933085739612579</v>
       </c>
       <c r="I36">
-        <v>0.001191423158161342</v>
+        <v>0.0008294502040371299</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37">
-        <v>127.5244553833956</v>
+        <v>116.6444537109252</v>
       </c>
       <c r="B37">
-        <v>0.1109043967041617</v>
+        <v>0.09544533930615096</v>
       </c>
       <c r="C37">
-        <v>0.0009876307296335129</v>
+        <v>0.0007694219399962561</v>
       </c>
       <c r="D37">
-        <v>0.6611051748588946</v>
+        <v>0.6631639025130645</v>
       </c>
       <c r="E37">
-        <v>1.031222090713138</v>
+        <v>1.032839738670361</v>
       </c>
       <c r="F37">
-        <v>72434.63899394819</v>
+        <v>94084.23138607158</v>
       </c>
       <c r="G37">
-        <v>127.8175659179688</v>
+        <v>115.7346572875977</v>
       </c>
       <c r="H37">
-        <v>0.1108576580882072</v>
+        <v>0.09672677516937256</v>
       </c>
       <c r="I37">
-        <v>0.0009856770047917962</v>
+        <v>0.0007734550163149834</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38">
-        <v>77.03922882308866</v>
+        <v>85.5653538607213</v>
       </c>
       <c r="B38">
-        <v>0.08664041627831462</v>
+        <v>0.1032812685196851</v>
       </c>
       <c r="C38">
-        <v>0.00124891785270003</v>
+        <v>0.001046284146412205</v>
       </c>
       <c r="D38">
-        <v>0.7721530584871934</v>
+        <v>0.7252779520285181</v>
       </c>
       <c r="E38">
-        <v>1.039508449645953</v>
+        <v>1.034038488018712</v>
       </c>
       <c r="F38">
-        <v>70038.58811791422</v>
+        <v>76929.58141154546</v>
       </c>
       <c r="G38">
-        <v>76.87385559082031</v>
+        <v>85.76645660400391</v>
       </c>
       <c r="H38">
-        <v>0.0869007483124733</v>
+        <v>0.104285441339016</v>
       </c>
       <c r="I38">
-        <v>0.001251642243005335</v>
+        <v>0.001044977805577219</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39">
-        <v>76.4202484116275</v>
+        <v>92.42878827595366</v>
       </c>
       <c r="B39">
-        <v>0.1014627886646332</v>
+        <v>0.08722309119517779</v>
       </c>
       <c r="C39">
-        <v>0.0007296093680730638</v>
+        <v>0.001117162003542812</v>
       </c>
       <c r="D39">
-        <v>0.7051391211988943</v>
+        <v>0.7538434285035041</v>
       </c>
       <c r="E39">
-        <v>1.036813073289158</v>
+        <v>1.035583928117089</v>
       </c>
       <c r="F39">
-        <v>108135.7357558151</v>
+        <v>75281.15860629341</v>
       </c>
       <c r="G39">
-        <v>76.80326080322266</v>
+        <v>93.54657745361328</v>
       </c>
       <c r="H39">
-        <v>0.1017491444945335</v>
+        <v>0.08647013455629349</v>
       </c>
       <c r="I39">
-        <v>0.0007276656688190997</v>
+        <v>0.001111424178816378</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40">
-        <v>105.381683380813</v>
+        <v>105.2559781117833</v>
       </c>
       <c r="B40">
-        <v>0.07704281765023344</v>
+        <v>0.1123944823763787</v>
       </c>
       <c r="C40">
-        <v>0.0008757331390162088</v>
+        <v>0.001103174284357493</v>
       </c>
       <c r="D40">
-        <v>0.7366798418087989</v>
+        <v>0.6962303051159605</v>
       </c>
       <c r="E40">
-        <v>1.036145897176781</v>
+        <v>1.030911798122509</v>
       </c>
       <c r="F40">
-        <v>93581.48987092268</v>
+        <v>68905.31545782315</v>
       </c>
       <c r="G40">
-        <v>106.6594848632812</v>
+        <v>103.0033264160156</v>
       </c>
       <c r="H40">
-        <v>0.0762021392583847</v>
+        <v>0.1136720106005669</v>
       </c>
       <c r="I40">
-        <v>0.0008709004032425582</v>
+        <v>0.001099986606277525</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41">
-        <v>114.7238844368376</v>
+        <v>86.36931414546802</v>
       </c>
       <c r="B41">
-        <v>0.07959071721125148</v>
+        <v>0.09489141216001384</v>
       </c>
       <c r="C41">
-        <v>0.0011290315584791</v>
+        <v>0.001269316612432304</v>
       </c>
       <c r="D41">
-        <v>0.7508367958983412</v>
+        <v>0.7518815301233097</v>
       </c>
       <c r="E41">
-        <v>1.034256297073972</v>
+        <v>1.035135543584959</v>
       </c>
       <c r="F41">
-        <v>73501.88707845574</v>
+        <v>66059.97446782426</v>
       </c>
       <c r="G41">
-        <v>116.6316070556641</v>
+        <v>86.70062255859375</v>
       </c>
       <c r="H41">
-        <v>0.08014797419309616</v>
+        <v>0.09520813822746277</v>
       </c>
       <c r="I41">
-        <v>0.001131046796217561</v>
+        <v>0.001268817228265107</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42">
-        <v>120.8890228208191</v>
+        <v>92.25116795307332</v>
       </c>
       <c r="B42">
-        <v>0.07280838128273133</v>
+        <v>0.09163273362915354</v>
       </c>
       <c r="C42">
-        <v>0.0009508655270488005</v>
+        <v>0.0007016219283361016</v>
       </c>
       <c r="D42">
-        <v>0.739061649744676</v>
+        <v>0.6934937734376011</v>
       </c>
       <c r="E42">
-        <v>1.035322645648141</v>
+        <v>1.03539229156198</v>
       </c>
       <c r="F42">
-        <v>85958.50187762419</v>
+        <v>109687.8970505162</v>
       </c>
       <c r="G42">
-        <v>109.4487686157227</v>
+        <v>89.21654510498047</v>
       </c>
       <c r="H42">
-        <v>0.07927943766117096</v>
+        <v>0.09423420578241348</v>
       </c>
       <c r="I42">
-        <v>0.0009533663978800178</v>
+        <v>0.0006963542546145618</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43">
-        <v>126.1499248130073</v>
+        <v>81.82325681113838</v>
       </c>
       <c r="B43">
-        <v>0.128243886566238</v>
+        <v>0.1197194148733443</v>
       </c>
       <c r="C43">
-        <v>0.0008037708125626938</v>
+        <v>0.001088317992336421</v>
       </c>
       <c r="D43">
-        <v>0.6029673937061979</v>
+        <v>0.7050034456610916</v>
       </c>
       <c r="E43">
-        <v>1.031530081986548</v>
+        <v>1.032468371488746</v>
       </c>
       <c r="F43">
-        <v>80746.29404517659</v>
+        <v>71505.63577606776</v>
       </c>
       <c r="G43">
-        <v>126.2087249755859</v>
+        <v>81.19797515869141</v>
       </c>
       <c r="H43">
-        <v>0.1271478831768036</v>
+        <v>0.120142862200737</v>
       </c>
       <c r="I43">
-        <v>0.0007987985736690462</v>
+        <v>0.001090904232114553</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44">
-        <v>129.0055745356385</v>
+        <v>97.59135302536043</v>
       </c>
       <c r="B44">
-        <v>0.07023162109061568</v>
+        <v>0.1254980147171915</v>
       </c>
       <c r="C44">
-        <v>0.0007643264472571276</v>
+        <v>0.001060235342258584</v>
       </c>
       <c r="D44">
-        <v>0.6998361324272053</v>
+        <v>0.6798198124465233</v>
       </c>
       <c r="E44">
-        <v>1.035658125287306</v>
+        <v>1.030364519758268</v>
       </c>
       <c r="F44">
-        <v>100794.3314531837</v>
+        <v>69935.79201984179</v>
       </c>
       <c r="G44">
-        <v>80.47441864013672</v>
+        <v>97.42069244384766</v>
       </c>
       <c r="H44">
-        <v>0.105047345161438</v>
+        <v>0.1252039968967438</v>
       </c>
       <c r="I44">
-        <v>0.0007690023048780859</v>
+        <v>0.001063338131643832</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45">
-        <v>93.98810153347155</v>
+        <v>72.67673807524685</v>
       </c>
       <c r="B45">
-        <v>0.08071479808345938</v>
+        <v>0.07276043865323782</v>
       </c>
       <c r="C45">
-        <v>0.001190403466876973</v>
+        <v>0.001053243765982173</v>
       </c>
       <c r="D45">
-        <v>0.7704451941239479</v>
+        <v>0.7960790197880054</v>
       </c>
       <c r="E45">
-        <v>1.036719414338063</v>
+        <v>1.046505445640872</v>
       </c>
       <c r="F45">
-        <v>72501.27757884889</v>
+        <v>87496.75459594239</v>
       </c>
       <c r="G45">
-        <v>93.89958190917969</v>
+        <v>68.28809356689453</v>
       </c>
       <c r="H45">
-        <v>0.08147343248128891</v>
+        <v>0.0740291103720665</v>
       </c>
       <c r="I45">
-        <v>0.001190944807603955</v>
+        <v>0.001079471199773252</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46">
-        <v>92.82011101165439</v>
+        <v>117.9877530742371</v>
       </c>
       <c r="B46">
-        <v>0.1067720051870195</v>
+        <v>0.08395761956978594</v>
       </c>
       <c r="C46">
-        <v>0.0009838857870793866</v>
+        <v>0.001277662191904146</v>
       </c>
       <c r="D46">
-        <v>0.7067630703690788</v>
+        <v>0.7509289033229314</v>
       </c>
       <c r="E46">
-        <v>1.032597290472734</v>
+        <v>1.033119127488469</v>
       </c>
       <c r="F46">
-        <v>79147.15046677139</v>
+        <v>64684.61011302021</v>
       </c>
       <c r="G46">
-        <v>102.3271331787109</v>
+        <v>120.1245040893555</v>
       </c>
       <c r="H46">
-        <v>0.1000404432415962</v>
+        <v>0.08241034299135208</v>
       </c>
       <c r="I46">
-        <v>0.0009781128028407693</v>
+        <v>0.001275137299671769</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47">
-        <v>78.86852060183634</v>
+        <v>74.61738681919796</v>
       </c>
       <c r="B47">
-        <v>0.07488217593119832</v>
+        <v>0.09091116216955381</v>
       </c>
       <c r="C47">
-        <v>0.001229370203151464</v>
+        <v>0.0007101230040220238</v>
       </c>
       <c r="D47">
-        <v>0.7946483901024534</v>
+        <v>0.7244274660794678</v>
       </c>
       <c r="E47">
-        <v>1.042722658883091</v>
+        <v>1.039774856525604</v>
       </c>
       <c r="F47">
-        <v>73986.15181765612</v>
+        <v>115268.2536515907</v>
       </c>
       <c r="G47">
-        <v>78.06148529052734</v>
+        <v>74.14821624755859</v>
       </c>
       <c r="H47">
-        <v>0.07532857358455658</v>
+        <v>0.09100337326526642</v>
       </c>
       <c r="I47">
-        <v>0.001226019929163158</v>
+        <v>0.0007023457437753677</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48">
-        <v>111.0960663210136</v>
+        <v>101.1301089298916</v>
       </c>
       <c r="B48">
-        <v>0.1229137901858099</v>
+        <v>0.1188979887622148</v>
       </c>
       <c r="C48">
-        <v>0.001139973480590036</v>
+        <v>0.00111788945842087</v>
       </c>
       <c r="D48">
-        <v>0.6777699228715108</v>
+        <v>0.6912449994477253</v>
       </c>
       <c r="E48">
-        <v>1.030043546053327</v>
+        <v>1.030575868810828</v>
       </c>
       <c r="F48">
-        <v>64519.41239221603</v>
+        <v>67486.50834535131</v>
       </c>
       <c r="G48">
-        <v>109.9700164794922</v>
+        <v>100.8356323242188</v>
       </c>
       <c r="H48">
-        <v>0.1233293190598488</v>
+        <v>0.1190713122487068</v>
       </c>
       <c r="I48">
-        <v>0.001138519961386919</v>
+        <v>0.00111280323471874</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49">
-        <v>109.4057175064502</v>
+        <v>88.40860597271177</v>
       </c>
       <c r="B49">
-        <v>0.1131772094705373</v>
+        <v>0.1291294856585979</v>
       </c>
       <c r="C49">
-        <v>0.0009458357233784461</v>
+        <v>0.001188207189821118</v>
       </c>
       <c r="D49">
-        <v>0.6727844373847738</v>
+        <v>0.6919086914895073</v>
       </c>
       <c r="E49">
-        <v>1.031008651106888</v>
+        <v>1.030659096815424</v>
       </c>
       <c r="F49">
-        <v>77450.65188049707</v>
+        <v>63765.16661566282</v>
       </c>
       <c r="G49">
-        <v>104.50537109375</v>
+        <v>113.6121444702148</v>
       </c>
       <c r="H49">
-        <v>0.1168106123805046</v>
+        <v>0.1137344166636467</v>
       </c>
       <c r="I49">
-        <v>0.0009459425345994532</v>
+        <v>0.001182602718472481</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50">
-        <v>121.7237557510724</v>
+        <v>104.6525769298825</v>
       </c>
       <c r="B50">
-        <v>0.1279833982862736</v>
+        <v>0.1281383022802211</v>
       </c>
       <c r="C50">
-        <v>0.0009241066084934102</v>
+        <v>0.00100588431797295</v>
       </c>
       <c r="D50">
-        <v>0.6319225437791637</v>
+        <v>0.6630887129205342</v>
       </c>
       <c r="E50">
-        <v>1.03064278021354</v>
+        <v>1.030076447969352</v>
       </c>
       <c r="F50">
-        <v>73766.93952127633</v>
+        <v>71593.2130990243</v>
       </c>
       <c r="G50">
-        <v>120.1783905029297</v>
+        <v>105.6736526489258</v>
       </c>
       <c r="H50">
-        <v>0.1280969828367233</v>
+        <v>0.1268824636936188</v>
       </c>
       <c r="I50">
-        <v>0.0009213577141053975</v>
+        <v>0.001009179861284792</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51">
-        <v>75.83547968725844</v>
+        <v>127.5660004500055</v>
       </c>
       <c r="B51">
-        <v>0.1004581328344459</v>
+        <v>0.1242969007329956</v>
       </c>
       <c r="C51">
-        <v>0.001009383007990751</v>
+        <v>0.0009003789217580855</v>
       </c>
       <c r="D51">
-        <v>0.7363906439594139</v>
+        <v>0.6259017067549253</v>
       </c>
       <c r="E51">
-        <v>1.036775740262979</v>
+        <v>1.031170570294291</v>
       </c>
       <c r="F51">
-        <v>81819.06652363189</v>
+        <v>74908.02692560162</v>
       </c>
       <c r="G51">
-        <v>74.73857116699219</v>
+        <v>127.101432800293</v>
       </c>
       <c r="H51">
-        <v>0.1014592573046684</v>
+        <v>0.1238811612129211</v>
       </c>
       <c r="I51">
-        <v>0.001001103431917727</v>
+        <v>0.0009009406203404069</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52">
-        <v>99.86661446952051</v>
+        <v>108.7342146673602</v>
       </c>
       <c r="B52">
-        <v>0.08802422098950924</v>
+        <v>0.0877933759038418</v>
       </c>
       <c r="C52">
-        <v>0.001233435971913837</v>
+        <v>0.001174504097936443</v>
       </c>
       <c r="D52">
-        <v>0.7537725012292393</v>
+        <v>0.7430311663603053</v>
       </c>
       <c r="E52">
-        <v>1.034186742051913</v>
+        <v>1.033340787225527</v>
       </c>
       <c r="F52">
-        <v>67783.98712820212</v>
+        <v>69789.22161430112</v>
       </c>
       <c r="G52">
-        <v>99.12236022949219</v>
+        <v>117.627067565918</v>
       </c>
       <c r="H52">
-        <v>0.08881272375583649</v>
+        <v>0.08367262035608292</v>
       </c>
       <c r="I52">
-        <v>0.001236436190083623</v>
+        <v>0.00117189809679985</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53">
-        <v>104.8649157803238</v>
+        <v>72.12174614532945</v>
       </c>
       <c r="B53">
-        <v>0.1029700343677163</v>
+        <v>0.1295206746048684</v>
       </c>
       <c r="C53">
-        <v>0.001142367147828501</v>
+        <v>0.0007583457553794547</v>
       </c>
       <c r="D53">
-        <v>0.7157282999257183</v>
+        <v>0.6713581517234944</v>
       </c>
       <c r="E53">
-        <v>1.031756100998037</v>
+        <v>1.033607528605515</v>
       </c>
       <c r="F53">
-        <v>68697.25871099719</v>
+        <v>98010.11850424354</v>
       </c>
       <c r="G53">
-        <v>106.0357666015625</v>
+        <v>107.6986312866211</v>
       </c>
       <c r="H53">
-        <v>0.1026739105582237</v>
+        <v>0.09707831591367722</v>
       </c>
       <c r="I53">
-        <v>0.001144547713920474</v>
+        <v>0.0007532954914495349</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54">
-        <v>84.49342240239511</v>
+        <v>95.82414637048367</v>
       </c>
       <c r="B54">
-        <v>0.1258491230378784</v>
+        <v>0.08496520246338708</v>
       </c>
       <c r="C54">
-        <v>0.0007030917785614139</v>
+        <v>0.0009652213826379551</v>
       </c>
       <c r="D54">
-        <v>0.6485887452622191</v>
+        <v>0.7420972316457739</v>
       </c>
       <c r="E54">
-        <v>1.032079238179593</v>
+        <v>1.035695301569764</v>
       </c>
       <c r="F54">
-        <v>101240.6048194076</v>
+        <v>85650.14209179072</v>
       </c>
       <c r="G54">
-        <v>88.47726440429688</v>
+        <v>98.50467681884766</v>
       </c>
       <c r="H54">
-        <v>0.1213109865784645</v>
+        <v>0.08392449468374252</v>
       </c>
       <c r="I54">
-        <v>0.0007105075637809932</v>
+        <v>0.0009616370662115514</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55">
-        <v>80.14152436774968</v>
+        <v>100.601011139095</v>
       </c>
       <c r="B55">
-        <v>0.1012456862345116</v>
+        <v>0.07635436929293393</v>
       </c>
       <c r="C55">
-        <v>0.001116494710821475</v>
+        <v>0.001011971424742503</v>
       </c>
       <c r="D55">
-        <v>0.737755870750154</v>
+        <v>0.7603713836825857</v>
       </c>
       <c r="E55">
-        <v>1.035422239189387</v>
+        <v>1.036827417593963</v>
       </c>
       <c r="F55">
-        <v>73769.6885288677</v>
+        <v>84004.68860621215</v>
       </c>
       <c r="G55">
-        <v>79.98193359375</v>
+        <v>100.8290557861328</v>
       </c>
       <c r="H55">
-        <v>0.1008702889084816</v>
+        <v>0.07603295892477036</v>
       </c>
       <c r="I55">
-        <v>0.001119478023611009</v>
+        <v>0.001008577062748373</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56">
-        <v>121.5748501851773</v>
+        <v>102.1706496822071</v>
       </c>
       <c r="B56">
-        <v>0.08603242191173913</v>
+        <v>0.1270571566633237</v>
       </c>
       <c r="C56">
-        <v>0.001251704444143492</v>
+        <v>0.001116373846560729</v>
       </c>
       <c r="D56">
-        <v>0.741850301843517</v>
+        <v>0.6780824810907395</v>
       </c>
       <c r="E56">
-        <v>1.032672393276567</v>
+        <v>1.030007417816073</v>
       </c>
       <c r="F56">
-        <v>65030.60797008016</v>
+        <v>66077.63294655208</v>
       </c>
       <c r="G56">
-        <v>117.3686904907227</v>
+        <v>102.3433609008789</v>
       </c>
       <c r="H56">
-        <v>0.08810614794492722</v>
+        <v>0.1268762648105621</v>
       </c>
       <c r="I56">
-        <v>0.001248170388862491</v>
+        <v>0.001117385225370526</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57">
-        <v>73.51209533413353</v>
+        <v>110.8835506362303</v>
       </c>
       <c r="B57">
-        <v>0.1226439273504472</v>
+        <v>0.08400521532808579</v>
       </c>
       <c r="C57">
-        <v>0.001126273455702695</v>
+        <v>0.0007545314392194457</v>
       </c>
       <c r="D57">
-        <v>0.7090537553834283</v>
+        <v>0.6916603426226564</v>
       </c>
       <c r="E57">
-        <v>1.0337350308076</v>
+        <v>1.034493140895126</v>
       </c>
       <c r="F57">
-        <v>69877.24966730582</v>
+        <v>100975.527628077</v>
       </c>
       <c r="G57">
-        <v>72.98419952392578</v>
+        <v>96.81012725830078</v>
       </c>
       <c r="H57">
-        <v>0.1223855316638947</v>
+        <v>0.09473104774951935</v>
       </c>
       <c r="I57">
-        <v>0.001125415554270148</v>
+        <v>0.000756004243157804</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58">
-        <v>98.23725423508438</v>
+        <v>86.65576586390597</v>
       </c>
       <c r="B58">
-        <v>0.09231512491074768</v>
+        <v>0.111386095904665</v>
       </c>
       <c r="C58">
-        <v>0.0008062034689404976</v>
+        <v>0.0008366557009227165</v>
       </c>
       <c r="D58">
-        <v>0.702897869144855</v>
+        <v>0.6893741094844896</v>
       </c>
       <c r="E58">
-        <v>1.034277135924389</v>
+        <v>1.033053102593614</v>
       </c>
       <c r="F58">
-        <v>96382.64012371401</v>
+        <v>90918.44856958336</v>
       </c>
       <c r="G58">
-        <v>97.47975921630859</v>
+        <v>96.1671142578125</v>
       </c>
       <c r="H58">
-        <v>0.09340403228998184</v>
+        <v>0.1037992238998413</v>
       </c>
       <c r="I58">
-        <v>0.0008067961316555738</v>
+        <v>0.0008358861086890101</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59">
-        <v>76.95004007805312</v>
+        <v>77.73163392797922</v>
       </c>
       <c r="B59">
-        <v>0.07008300099993997</v>
+        <v>0.07350138153883533</v>
       </c>
       <c r="C59">
-        <v>0.0009901108764564753</v>
+        <v>0.0009461809376140754</v>
       </c>
       <c r="D59">
-        <v>0.7952391543879603</v>
+        <v>0.7836174803134465</v>
       </c>
       <c r="E59">
-        <v>1.045809569639264</v>
+        <v>1.044026492201375</v>
       </c>
       <c r="F59">
-        <v>92726.65505905832</v>
+        <v>95051.63922418877</v>
       </c>
       <c r="G59">
-        <v>71.77478790283203</v>
+        <v>77.61281585693359</v>
       </c>
       <c r="H59">
-        <v>0.07143482565879822</v>
+        <v>0.07260549068450928</v>
       </c>
       <c r="I59">
-        <v>0.001002095523290336</v>
+        <v>0.0009546757792122662</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60">
-        <v>97.42352567988203</v>
+        <v>93.56054059282566</v>
       </c>
       <c r="B60">
-        <v>0.08486110134953896</v>
+        <v>0.1138425459476486</v>
       </c>
       <c r="C60">
-        <v>0.0007841896107540516</v>
+        <v>0.001073976803812078</v>
       </c>
       <c r="D60">
-        <v>0.7153575000305042</v>
+        <v>0.7025655854041015</v>
       </c>
       <c r="E60">
-        <v>1.035759001392109</v>
+        <v>1.031611943632618</v>
       </c>
       <c r="F60">
-        <v>101383.3216051622</v>
+        <v>71826.831781958</v>
       </c>
       <c r="G60">
-        <v>102.1681137084961</v>
+        <v>107.0227203369141</v>
       </c>
       <c r="H60">
-        <v>0.08100271224975586</v>
+        <v>0.1050769686698914</v>
       </c>
       <c r="I60">
-        <v>0.0007840448524802923</v>
+        <v>0.00106576515827328</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61">
-        <v>128.7977395805385</v>
+        <v>127.3843433677569</v>
       </c>
       <c r="B61">
-        <v>0.08909401055062374</v>
+        <v>0.1229032127400304</v>
       </c>
       <c r="C61">
-        <v>0.0009153971670037792</v>
+        <v>0.00123217646873045</v>
       </c>
       <c r="D61">
-        <v>0.6878981894309247</v>
+        <v>0.6712267614482742</v>
       </c>
       <c r="E61">
-        <v>1.032845146076316</v>
+        <v>1.030162139747776</v>
       </c>
       <c r="F61">
-        <v>81936.40473166673</v>
+        <v>58792.79863789047</v>
       </c>
       <c r="G61">
-        <v>102.4431915283203</v>
+        <v>126.699951171875</v>
       </c>
       <c r="H61">
-        <v>0.1083281114697456</v>
+        <v>0.1225026473402977</v>
       </c>
       <c r="I61">
-        <v>0.000920608697924763</v>
+        <v>0.001232064561918378</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62">
-        <v>95.42238120732837</v>
+        <v>81.22785350505069</v>
       </c>
       <c r="B62">
-        <v>0.1215266480939141</v>
+        <v>0.08634621372795775</v>
       </c>
       <c r="C62">
-        <v>0.001262270225164311</v>
+        <v>0.001071295700944826</v>
       </c>
       <c r="D62">
-        <v>0.7016740500078656</v>
+        <v>0.7619058217169913</v>
       </c>
       <c r="E62">
-        <v>1.03058134424215</v>
+        <v>1.03841754716077</v>
       </c>
       <c r="F62">
-        <v>60800.40810153226</v>
+        <v>80204.54288786212</v>
       </c>
       <c r="G62">
-        <v>108.2312088012695</v>
+        <v>81.16973114013672</v>
       </c>
       <c r="H62">
-        <v>0.1145538985729218</v>
+        <v>0.08642566204071045</v>
       </c>
       <c r="I62">
-        <v>0.001255246577784419</v>
+        <v>0.001064303447492421</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63">
-        <v>121.427495050274</v>
+        <v>124.2390372956942</v>
       </c>
       <c r="B63">
-        <v>0.0975101900239867</v>
+        <v>0.09274341376464572</v>
       </c>
       <c r="C63">
-        <v>0.001253983184535225</v>
+        <v>0.0007800768825609606</v>
       </c>
       <c r="D63">
-        <v>0.7200631229204343</v>
+        <v>0.659786208627306</v>
       </c>
       <c r="E63">
-        <v>1.031445803271471</v>
+        <v>1.032969699070241</v>
       </c>
       <c r="F63">
-        <v>62647.39736035832</v>
+        <v>92131.06854128822</v>
       </c>
       <c r="G63">
-        <v>112.301139831543</v>
+        <v>123.0698471069336</v>
       </c>
       <c r="H63">
-        <v>0.1020333617925644</v>
+        <v>0.09268553555011749</v>
       </c>
       <c r="I63">
-        <v>0.001256656367331743</v>
+        <v>0.0007814713171683252</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64">
-        <v>77.03893385099164</v>
+        <v>102.6283570046396</v>
       </c>
       <c r="B64">
-        <v>0.09667523726867805</v>
+        <v>0.09245777099925498</v>
       </c>
       <c r="C64">
-        <v>0.0008697021113056497</v>
+        <v>0.001288348079672369</v>
       </c>
       <c r="D64">
-        <v>0.7305748892924614</v>
+        <v>0.7464108438955319</v>
       </c>
       <c r="E64">
-        <v>1.0373935757557</v>
+        <v>1.033112754894964</v>
       </c>
       <c r="F64">
-        <v>94312.37796708505</v>
+        <v>63972.11208752811</v>
       </c>
       <c r="G64">
-        <v>76.17283630371094</v>
+        <v>101.3477554321289</v>
       </c>
       <c r="H64">
-        <v>0.09731194376945496</v>
+        <v>0.09273909777402878</v>
       </c>
       <c r="I64">
-        <v>0.0008659679442644119</v>
+        <v>0.001278837444260716</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65">
-        <v>86.27512460571185</v>
+        <v>97.41468529874595</v>
       </c>
       <c r="B65">
-        <v>0.09016613598399326</v>
+        <v>0.114927295452408</v>
       </c>
       <c r="C65">
-        <v>0.0009037786264997194</v>
+        <v>0.001223071440853296</v>
       </c>
       <c r="D65">
-        <v>0.7357543114695229</v>
+        <v>0.7080071533641324</v>
       </c>
       <c r="E65">
-        <v>1.036480328452593</v>
+        <v>1.031032946151278</v>
       </c>
       <c r="F65">
-        <v>91032.41378563996</v>
+        <v>63405.36262171731</v>
       </c>
       <c r="G65">
-        <v>85.928955078125</v>
+        <v>109.5109176635742</v>
       </c>
       <c r="H65">
-        <v>0.09059428423643112</v>
+        <v>0.1085422188043594</v>
       </c>
       <c r="I65">
-        <v>0.0008999753626994789</v>
+        <v>0.001223067403770983</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66">
-        <v>94.22756444004008</v>
+        <v>122.9224846137934</v>
       </c>
       <c r="B66">
-        <v>0.1228406873828248</v>
+        <v>0.08426843455234234</v>
       </c>
       <c r="C66">
-        <v>0.001060127720878776</v>
+        <v>0.001001632456687194</v>
       </c>
       <c r="D66">
-        <v>0.6870354194766125</v>
+        <v>0.7180551658842926</v>
       </c>
       <c r="E66">
-        <v>1.030766603696143</v>
+        <v>1.033268379973316</v>
       </c>
       <c r="F66">
-        <v>70876.83645246296</v>
+        <v>78613.77367316131</v>
       </c>
       <c r="G66">
-        <v>99.63333892822266</v>
+        <v>110.1783828735352</v>
       </c>
       <c r="H66">
-        <v>0.1193309277296066</v>
+        <v>0.09101053327322006</v>
       </c>
       <c r="I66">
-        <v>0.001058234367519617</v>
+        <v>0.000999326934106648</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67">
-        <v>93.98872840055984</v>
+        <v>97.51623770611515</v>
       </c>
       <c r="B67">
-        <v>0.1267016066164235</v>
+        <v>0.08031118594285859</v>
       </c>
       <c r="C67">
-        <v>0.001277918377156228</v>
+        <v>0.00125340878907798</v>
       </c>
       <c r="D67">
-        <v>0.6959994828893421</v>
+        <v>0.7722417368705079</v>
       </c>
       <c r="E67">
-        <v>1.030307595402386</v>
+        <v>1.036113607922656</v>
       </c>
       <c r="F67">
-        <v>59507.28083689478</v>
+        <v>68854.52178132093</v>
       </c>
       <c r="G67">
-        <v>109.5108261108398</v>
+        <v>97.73268127441406</v>
       </c>
       <c r="H67">
-        <v>0.1183531135320663</v>
+        <v>0.08070660382509232</v>
       </c>
       <c r="I67">
-        <v>0.001268908148631454</v>
+        <v>0.001249604043550789</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68">
-        <v>110.2830087202092</v>
+        <v>113.4500581966926</v>
       </c>
       <c r="B68">
-        <v>0.1295134197492778</v>
+        <v>0.0969574989212643</v>
       </c>
       <c r="C68">
-        <v>0.0007886808004392343</v>
+        <v>0.001024828476254281</v>
       </c>
       <c r="D68">
-        <v>0.6205977362955652</v>
+        <v>0.7062920070955223</v>
       </c>
       <c r="E68">
-        <v>1.030720768159888</v>
+        <v>1.03210422635024</v>
       </c>
       <c r="F68">
-        <v>85139.37817486007</v>
+        <v>75426.70490275986</v>
       </c>
       <c r="G68">
-        <v>109.0429382324219</v>
+        <v>103.5700454711914</v>
       </c>
       <c r="H68">
-        <v>0.1301527619361877</v>
+        <v>0.102689690887928</v>
       </c>
       <c r="I68">
-        <v>0.0007876453455537558</v>
+        <v>0.001021251315250993</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69">
-        <v>90.68308764253047</v>
+        <v>93.94151930218612</v>
       </c>
       <c r="B69">
-        <v>0.09260447601765921</v>
+        <v>0.08826810444263918</v>
       </c>
       <c r="C69">
-        <v>0.0008541499862120014</v>
+        <v>0.001253983640733498</v>
       </c>
       <c r="D69">
-        <v>0.7197115853229062</v>
+        <v>0.7586722341541576</v>
       </c>
       <c r="E69">
-        <v>1.035234983887674</v>
+        <v>1.035012386868168</v>
       </c>
       <c r="F69">
-        <v>93686.10793409534</v>
+        <v>67379.26100820751</v>
       </c>
       <c r="G69">
-        <v>105.5469055175781</v>
+        <v>94.77121734619141</v>
       </c>
       <c r="H69">
-        <v>0.0826667845249176</v>
+        <v>0.08809309452772141</v>
       </c>
       <c r="I69">
-        <v>0.0008467088919132948</v>
+        <v>0.001251145149581134</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70">
-        <v>112.826012104601</v>
+        <v>124.2426635740575</v>
       </c>
       <c r="B70">
-        <v>0.1279688467376303</v>
+        <v>0.1203513473355191</v>
       </c>
       <c r="C70">
-        <v>0.001224134096374463</v>
+        <v>0.001197938421162006</v>
       </c>
       <c r="D70">
-        <v>0.6759704116954021</v>
+        <v>0.6747090725877974</v>
       </c>
       <c r="E70">
-        <v>1.029642123796905</v>
+        <v>1.030195660305991</v>
       </c>
       <c r="F70">
-        <v>59807.79180488024</v>
+        <v>60884.78636189843</v>
       </c>
       <c r="G70">
-        <v>110.032112121582</v>
+        <v>123.880744934082</v>
       </c>
       <c r="H70">
-        <v>0.1295935362577438</v>
+        <v>0.1202794015407562</v>
       </c>
       <c r="I70">
-        <v>0.001218904624693096</v>
+        <v>0.001199990045279264</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71">
-        <v>108.3512139535235</v>
+        <v>111.4015012114736</v>
       </c>
       <c r="B71">
-        <v>0.1175127741778541</v>
+        <v>0.08426450956093834</v>
       </c>
       <c r="C71">
-        <v>0.0009951353390250067</v>
+        <v>0.001280971846176578</v>
       </c>
       <c r="D71">
-        <v>0.6735316551968298</v>
+        <v>0.7555827568877244</v>
       </c>
       <c r="E71">
-        <v>1.030639143358266</v>
+        <v>1.033554997771391</v>
       </c>
       <c r="F71">
-        <v>73632.63088688425</v>
+        <v>65132.53743818783</v>
       </c>
       <c r="G71">
-        <v>105.0449905395508</v>
+        <v>114.4340515136719</v>
       </c>
       <c r="H71">
-        <v>0.1200704202055931</v>
+        <v>0.08334340900182724</v>
       </c>
       <c r="I71">
-        <v>0.0009958785958588123</v>
+        <v>0.001278484123758972</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72">
-        <v>93.94966871528638</v>
+        <v>111.977323255031</v>
       </c>
       <c r="B72">
-        <v>0.110541348858656</v>
+        <v>0.1001433674493557</v>
       </c>
       <c r="C72">
-        <v>0.001239376655336219</v>
+        <v>0.001251869686466895</v>
       </c>
       <c r="D72">
-        <v>0.7185133410622222</v>
+        <v>0.7229529440166833</v>
       </c>
       <c r="E72">
-        <v>1.03177069477836</v>
+        <v>1.031516000110318</v>
       </c>
       <c r="F72">
-        <v>63746.79335910102</v>
+        <v>63192.24238684704</v>
       </c>
       <c r="G72">
-        <v>102.9731140136719</v>
+        <v>110.8038330078125</v>
       </c>
       <c r="H72">
-        <v>0.1066054850816727</v>
+        <v>0.1010221615433693</v>
       </c>
       <c r="I72">
-        <v>0.00123877392616123</v>
+        <v>0.001251667155884206</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73">
-        <v>95.90560765925915</v>
+        <v>89.66322409342713</v>
       </c>
       <c r="B73">
-        <v>0.08469336876520597</v>
+        <v>0.1265550159818758</v>
       </c>
       <c r="C73">
-        <v>0.0008113107385139058</v>
+        <v>0.0007216202904571417</v>
       </c>
       <c r="D73">
-        <v>0.7223852437768853</v>
+        <v>0.6428400718666736</v>
       </c>
       <c r="E73">
-        <v>1.035978014498051</v>
+        <v>1.031500650984298</v>
       </c>
       <c r="F73">
-        <v>99110.88441039556</v>
+        <v>97423.08144292615</v>
       </c>
       <c r="G73">
-        <v>103.1757888793945</v>
+        <v>91.79714965820312</v>
       </c>
       <c r="H73">
-        <v>0.07896748185157776</v>
+        <v>0.1234357953071594</v>
       </c>
       <c r="I73">
-        <v>0.0008106106542982161</v>
+        <v>0.0007213327335193753</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74">
-        <v>106.8716619886193</v>
+        <v>115.4067185642133</v>
       </c>
       <c r="B74">
-        <v>0.08298743565665259</v>
+        <v>0.1080398618646796</v>
       </c>
       <c r="C74">
-        <v>0.001019601152482816</v>
+        <v>0.000804863202496564</v>
       </c>
       <c r="D74">
-        <v>0.740303439347461</v>
+        <v>0.6497607976419914</v>
       </c>
       <c r="E74">
-        <v>1.034539950031452</v>
+        <v>1.031774069769799</v>
       </c>
       <c r="F74">
-        <v>80399.30772617376</v>
+        <v>87751.4399838269</v>
       </c>
       <c r="G74">
-        <v>113.6841506958008</v>
+        <v>117.1833419799805</v>
       </c>
       <c r="H74">
-        <v>0.0802156925201416</v>
+        <v>0.1062835603952408</v>
       </c>
       <c r="I74">
-        <v>0.00101686455309391</v>
+        <v>0.0008075246005319059</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75">
-        <v>74.20253140867868</v>
+        <v>108.1636633268285</v>
       </c>
       <c r="B75">
-        <v>0.07996286947127475</v>
+        <v>0.1220373643277479</v>
       </c>
       <c r="C75">
-        <v>0.0008957617795896235</v>
+        <v>0.0009334808062607114</v>
       </c>
       <c r="D75">
-        <v>0.7689674861784427</v>
+        <v>0.6587869851820719</v>
       </c>
       <c r="E75">
-        <v>1.043049053587333</v>
+        <v>1.030538061481173</v>
       </c>
       <c r="F75">
-        <v>98209.31680748955</v>
+        <v>76651.40706171868</v>
       </c>
       <c r="G75">
-        <v>71.90023803710938</v>
+        <v>108.4021606445312</v>
       </c>
       <c r="H75">
-        <v>0.08134298026561737</v>
+        <v>0.1220237836241722</v>
       </c>
       <c r="I75">
-        <v>0.0009030126384459436</v>
+        <v>0.0009304698905907571</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76">
-        <v>119.3444043013414</v>
+        <v>84.40121640278258</v>
       </c>
       <c r="B76">
-        <v>0.1253653966135219</v>
+        <v>0.1264125813612861</v>
       </c>
       <c r="C76">
-        <v>0.0008899255359354856</v>
+        <v>0.001271285618377252</v>
       </c>
       <c r="D76">
-        <v>0.6330084944063089</v>
+        <v>0.7024846697710218</v>
       </c>
       <c r="E76">
-        <v>1.030755158325317</v>
+        <v>1.031312108703894</v>
       </c>
       <c r="F76">
-        <v>76831.71262548529</v>
+        <v>60725.82533805999</v>
       </c>
       <c r="G76">
-        <v>117.9119415283203</v>
+        <v>83.57718658447266</v>
       </c>
       <c r="H76">
-        <v>0.1257322430610657</v>
+        <v>0.1276964992284775</v>
       </c>
       <c r="I76">
-        <v>0.0008864194387570024</v>
+        <v>0.001262687030248344</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77">
-        <v>109.2052696668182</v>
+        <v>79.63232934911538</v>
       </c>
       <c r="B77">
-        <v>0.08764459974298996</v>
+        <v>0.1150458917131811</v>
       </c>
       <c r="C77">
-        <v>0.0009681261783677194</v>
+        <v>0.0008800173516855577</v>
       </c>
       <c r="D77">
-        <v>0.7220785565286042</v>
+        <v>0.6975137278319087</v>
       </c>
       <c r="E77">
-        <v>1.033628973032096</v>
+        <v>1.033656499373038</v>
       </c>
       <c r="F77">
-        <v>82201.18354226797</v>
+        <v>87798.27856285183</v>
       </c>
       <c r="G77">
-        <v>106.1610565185547</v>
+        <v>103.4982452392578</v>
       </c>
       <c r="H77">
-        <v>0.09034965932369232</v>
+        <v>0.09825064986944199</v>
       </c>
       <c r="I77">
-        <v>0.0009696384076960385</v>
+        <v>0.0008709487738087773</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78">
-        <v>113.5805478650701</v>
+        <v>117.7834884710399</v>
       </c>
       <c r="B78">
-        <v>0.09718565472693272</v>
+        <v>0.1119745036134851</v>
       </c>
       <c r="C78">
-        <v>0.000959846469460761</v>
+        <v>0.0007962805863325608</v>
       </c>
       <c r="D78">
-        <v>0.6974252086273918</v>
+        <v>0.6380494264821477</v>
       </c>
       <c r="E78">
-        <v>1.032195846360961</v>
+        <v>1.031623369312156</v>
       </c>
       <c r="F78">
-        <v>79486.26041960322</v>
+        <v>86887.89637657868</v>
       </c>
       <c r="G78">
-        <v>102.2858505249023</v>
+        <v>118.4355697631836</v>
       </c>
       <c r="H78">
-        <v>0.1046614423394203</v>
+        <v>0.1113461852073669</v>
       </c>
       <c r="I78">
-        <v>0.000963313621468842</v>
+        <v>0.0007965444237925112</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79">
-        <v>102.2153800649434</v>
+        <v>127.5499961821133</v>
       </c>
       <c r="B79">
-        <v>0.09963747003923341</v>
+        <v>0.1280779339962536</v>
       </c>
       <c r="C79">
-        <v>0.0009144081278067726</v>
+        <v>0.001231782799651936</v>
       </c>
       <c r="D79">
-        <v>0.7003157765725175</v>
+        <v>0.663494792470514</v>
       </c>
       <c r="E79">
-        <v>1.032682037897726</v>
+        <v>1.030021348317159</v>
       </c>
       <c r="F79">
-        <v>84169.10097053806</v>
+        <v>58055.59213535698</v>
       </c>
       <c r="G79">
-        <v>102.0933380126953</v>
+        <v>126.9689178466797</v>
       </c>
       <c r="H79">
-        <v>0.09948776662349701</v>
+        <v>0.1270870566368103</v>
       </c>
       <c r="I79">
-        <v>0.000916847144253552</v>
+        <v>0.001225610030815005</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80">
-        <v>76.62862665950469</v>
+        <v>97.48832963560257</v>
       </c>
       <c r="B80">
-        <v>0.1166902957270153</v>
+        <v>0.1296640473788608</v>
       </c>
       <c r="C80">
-        <v>0.001248982462189371</v>
+        <v>0.0009678366492899215</v>
       </c>
       <c r="D80">
-        <v>0.7206819979920019</v>
+        <v>0.6646525516619286</v>
       </c>
       <c r="E80">
-        <v>1.033756040737481</v>
+        <v>1.030267758151803</v>
       </c>
       <c r="F80">
-        <v>64060.52365112171</v>
+        <v>74789.47468334551</v>
       </c>
       <c r="G80">
-        <v>76.60614013671875</v>
+        <v>100.4697952270508</v>
       </c>
       <c r="H80">
-        <v>0.1170766353607178</v>
+        <v>0.1266215592622757</v>
       </c>
       <c r="I80">
-        <v>0.001246946398168802</v>
+        <v>0.000970394117757678</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81">
-        <v>94.302136797817</v>
+        <v>105.4590499194211</v>
       </c>
       <c r="B81">
-        <v>0.1206540976931814</v>
+        <v>0.09710930096018558</v>
       </c>
       <c r="C81">
-        <v>0.001139046511259736</v>
+        <v>0.001244725356612596</v>
       </c>
       <c r="D81">
-        <v>0.6963221414745223</v>
+        <v>0.7330830737762567</v>
       </c>
       <c r="E81">
-        <v>1.030859552072446</v>
+        <v>1.032261482981537</v>
       </c>
       <c r="F81">
-        <v>66917.33520767967</v>
+        <v>64754.30163603505</v>
       </c>
       <c r="G81">
-        <v>104.0646896362305</v>
+        <v>115.8182373046875</v>
       </c>
       <c r="H81">
-        <v>0.1150055974721909</v>
+        <v>0.09213313460350037</v>
       </c>
       <c r="I81">
-        <v>0.001137807965278625</v>
+        <v>0.001237516873516142</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82">
-        <v>94.32241497091337</v>
+        <v>121.4633586516133</v>
       </c>
       <c r="B82">
-        <v>0.07834436206891678</v>
+        <v>0.0742521866910525</v>
       </c>
       <c r="C82">
-        <v>0.001136528194798918</v>
+        <v>0.0007961382797920859</v>
       </c>
       <c r="D82">
-        <v>0.7718915399280692</v>
+        <v>0.7076015334308489</v>
       </c>
       <c r="E82">
-        <v>1.037313167835007</v>
+        <v>1.035264297895054</v>
       </c>
       <c r="F82">
-        <v>76211.84154469764</v>
+        <v>98000.1974113451</v>
       </c>
       <c r="G82">
-        <v>94.12310791015625</v>
+        <v>103.5165023803711</v>
       </c>
       <c r="H82">
-        <v>0.07913605868816376</v>
+        <v>0.08528075367212296</v>
       </c>
       <c r="I82">
-        <v>0.001135451719164848</v>
+        <v>0.0007972652674652636</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83">
-        <v>89.26257940259302</v>
+        <v>97.43340720123143</v>
       </c>
       <c r="B83">
-        <v>0.09561426161266443</v>
+        <v>0.08756764188643114</v>
       </c>
       <c r="C83">
-        <v>0.0008739480697551733</v>
+        <v>0.00109667050690486</v>
       </c>
       <c r="D83">
-        <v>0.7183531697623106</v>
+        <v>0.7472935097252533</v>
       </c>
       <c r="E83">
-        <v>1.034896914913591</v>
+        <v>1.034755206113849</v>
       </c>
       <c r="F83">
-        <v>91325.56848006879</v>
+        <v>75711.33298290735</v>
       </c>
       <c r="G83">
-        <v>106.8002014160156</v>
+        <v>98.69664764404297</v>
       </c>
       <c r="H83">
-        <v>0.08425910770893097</v>
+        <v>0.08763977140188217</v>
       </c>
       <c r="I83">
-        <v>0.0008641164167784154</v>
+        <v>0.001090719480998814</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84">
-        <v>71.79701949428497</v>
+        <v>127.1124686099642</v>
       </c>
       <c r="B84">
-        <v>0.1205712932701274</v>
+        <v>0.07914128234126383</v>
       </c>
       <c r="C84">
-        <v>0.001046625654590104</v>
+        <v>0.0009641582516976951</v>
       </c>
       <c r="D84">
-        <v>0.7095654637969709</v>
+        <v>0.7191205321142327</v>
       </c>
       <c r="E84">
-        <v>1.034476064584767</v>
+        <v>1.033882001754481</v>
       </c>
       <c r="F84">
-        <v>75441.34946248977</v>
+        <v>81860.38508093773</v>
       </c>
       <c r="G84">
-        <v>71.73715209960938</v>
+        <v>109.9008483886719</v>
       </c>
       <c r="H84">
-        <v>0.1206203624606133</v>
+        <v>0.08845176547765732</v>
       </c>
       <c r="I84">
-        <v>0.001044698292389512</v>
+        <v>0.0009644533856771886</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85">
-        <v>114.2352545557886</v>
+        <v>104.5450697226923</v>
       </c>
       <c r="B85">
-        <v>0.1190819983453503</v>
+        <v>0.09504918248776072</v>
       </c>
       <c r="C85">
-        <v>0.001167507659981101</v>
+        <v>0.0007458920614181712</v>
       </c>
       <c r="D85">
-        <v>0.6830629939637342</v>
+        <v>0.6769168115460589</v>
       </c>
       <c r="E85">
-        <v>1.030179124835699</v>
+        <v>1.033442156556343</v>
       </c>
       <c r="F85">
-        <v>63490.12553397731</v>
+        <v>99705.66345280567</v>
       </c>
       <c r="G85">
-        <v>111.4974594116211</v>
+        <v>89.96017456054688</v>
       </c>
       <c r="H85">
-        <v>0.1203430518507957</v>
+        <v>0.1071885600686073</v>
       </c>
       <c r="I85">
-        <v>0.001168973161838949</v>
+        <v>0.0007444145740009844</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86">
-        <v>76.58706748375005</v>
+        <v>119.2460272420789</v>
       </c>
       <c r="B86">
-        <v>0.07614482550714499</v>
+        <v>0.07787735970839536</v>
       </c>
       <c r="C86">
-        <v>0.001177354221125928</v>
+        <v>0.0011178778867915</v>
       </c>
       <c r="D86">
-        <v>0.791371545217794</v>
+        <v>0.7493031809041089</v>
       </c>
       <c r="E86">
-        <v>1.043176772198835</v>
+        <v>1.034231366054525</v>
       </c>
       <c r="F86">
-        <v>77041.27100917042</v>
+        <v>73985.46036064232</v>
       </c>
       <c r="G86">
-        <v>75.12838745117188</v>
+        <v>118.6949615478516</v>
       </c>
       <c r="H86">
-        <v>0.07689573615789413</v>
+        <v>0.07814127951860428</v>
       </c>
       <c r="I86">
-        <v>0.001176573685370386</v>
+        <v>0.001122008659876883</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87">
-        <v>106.3784879827051</v>
+        <v>124.5306231047643</v>
       </c>
       <c r="B87">
-        <v>0.07938300093207779</v>
+        <v>0.1062470682412529</v>
       </c>
       <c r="C87">
-        <v>0.0009067182764525872</v>
+        <v>0.0008484392533234922</v>
       </c>
       <c r="D87">
-        <v>0.7346907753429761</v>
+        <v>0.6489240793419687</v>
       </c>
       <c r="E87">
-        <v>1.035472057678785</v>
+        <v>1.031857857747401</v>
       </c>
       <c r="F87">
-        <v>89931.80489764991</v>
+        <v>82911.49300625132</v>
       </c>
       <c r="G87">
-        <v>107.0807418823242</v>
+        <v>126.2307891845703</v>
       </c>
       <c r="H87">
-        <v>0.07957113534212112</v>
+        <v>0.1043998897075653</v>
       </c>
       <c r="I87">
-        <v>0.0009079063311219215</v>
+        <v>0.0008459447999484837</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88">
-        <v>112.1930497880329</v>
+        <v>118.9314291261141</v>
       </c>
       <c r="B88">
-        <v>0.08825192149596446</v>
+        <v>0.09296848354947125</v>
       </c>
       <c r="C88">
-        <v>0.001162523653941189</v>
+        <v>0.0007237693135477107</v>
       </c>
       <c r="D88">
-        <v>0.7381123390199201</v>
+        <v>0.6537500980346327</v>
       </c>
       <c r="E88">
-        <v>1.033015814612571</v>
+        <v>1.033183935486881</v>
       </c>
       <c r="F88">
-        <v>69886.77950814713</v>
+        <v>98551.80779565249</v>
       </c>
       <c r="G88">
-        <v>112.7958297729492</v>
+        <v>120.7478713989258</v>
       </c>
       <c r="H88">
-        <v>0.08887942880392075</v>
+        <v>0.09214907139539719</v>
       </c>
       <c r="I88">
-        <v>0.001161974621936679</v>
+        <v>0.0007288310443982482</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89">
-        <v>108.0871793760217</v>
+        <v>79.56486780693736</v>
       </c>
       <c r="B89">
-        <v>0.07452154414500042</v>
+        <v>0.1237231530572926</v>
       </c>
       <c r="C89">
-        <v>0.00114153633808464</v>
+        <v>0.0007359665789497439</v>
       </c>
       <c r="D89">
-        <v>0.7691292899537185</v>
+        <v>0.6653825927819952</v>
       </c>
       <c r="E89">
-        <v>1.036004964722029</v>
+        <v>1.032897020133581</v>
       </c>
       <c r="F89">
-        <v>75077.80795187084</v>
+        <v>99692.37878978255</v>
       </c>
       <c r="G89">
-        <v>108.3677139282227</v>
+        <v>90.73977661132812</v>
       </c>
       <c r="H89">
-        <v>0.07455265522003174</v>
+        <v>0.1117541939020157</v>
       </c>
       <c r="I89">
-        <v>0.001142293564043939</v>
+        <v>0.0007337864954024553</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90">
-        <v>127.5485351186785</v>
+        <v>107.733906343702</v>
       </c>
       <c r="B90">
-        <v>0.09547978017043558</v>
+        <v>0.1280676803079101</v>
       </c>
       <c r="C90">
-        <v>0.0007849038913731401</v>
+        <v>0.0007366471222400724</v>
       </c>
       <c r="D90">
-        <v>0.6508492479377164</v>
+        <v>0.615397816468679</v>
       </c>
       <c r="E90">
-        <v>1.032720088057245</v>
+        <v>1.030946857742948</v>
       </c>
       <c r="F90">
-        <v>90106.18543839187</v>
+        <v>90484.49204210629</v>
       </c>
       <c r="G90">
-        <v>124.4841842651367</v>
+        <v>106.9417724609375</v>
       </c>
       <c r="H90">
-        <v>0.09686605632305145</v>
+        <v>0.127449631690979</v>
       </c>
       <c r="I90">
-        <v>0.0007861975464038551</v>
+        <v>0.0007353218970820308</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91">
-        <v>76.19788930510832</v>
+        <v>93.90605551718062</v>
       </c>
       <c r="B91">
-        <v>0.07645706230897492</v>
+        <v>0.1028130941001653</v>
       </c>
       <c r="C91">
-        <v>0.001219567281139886</v>
+        <v>0.001244639774491023</v>
       </c>
       <c r="D91">
-        <v>0.7924240861125591</v>
+        <v>0.7316708220100967</v>
       </c>
       <c r="E91">
-        <v>1.043186739430791</v>
+        <v>1.032690574326936</v>
       </c>
       <c r="F91">
-        <v>74486.43958519514</v>
+        <v>64886.20240510526</v>
       </c>
       <c r="G91">
-        <v>74.87374114990234</v>
+        <v>93.87107086181641</v>
       </c>
       <c r="H91">
-        <v>0.07722079008817673</v>
+        <v>0.1033591330051422</v>
       </c>
       <c r="I91">
-        <v>0.00121659878641367</v>
+        <v>0.00124220282305032</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92">
-        <v>122.030029546312</v>
+        <v>73.76277712140075</v>
       </c>
       <c r="B92">
-        <v>0.1040930556201907</v>
+        <v>0.0864894141920558</v>
       </c>
       <c r="C92">
-        <v>0.0009647928821082464</v>
+        <v>0.001143930350697461</v>
       </c>
       <c r="D92">
-        <v>0.6757118671480584</v>
+        <v>0.7706444681855789</v>
       </c>
       <c r="E92">
-        <v>1.0315330772985</v>
+        <v>1.040790254014559</v>
       </c>
       <c r="F92">
-        <v>76110.79029304822</v>
+        <v>76623.29227965612</v>
       </c>
       <c r="G92">
-        <v>122.3652267456055</v>
+        <v>74.44188690185547</v>
       </c>
       <c r="H92">
-        <v>0.1035260409116745</v>
+        <v>0.08592323213815689</v>
       </c>
       <c r="I92">
-        <v>0.0009601544006727636</v>
+        <v>0.001142060966230929</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93">
-        <v>71.7514140909348</v>
+        <v>95.44193511339051</v>
       </c>
       <c r="B93">
-        <v>0.08479341638866937</v>
+        <v>0.1055338251257102</v>
       </c>
       <c r="C93">
-        <v>0.0009918462693331992</v>
+        <v>0.001238837414328241</v>
       </c>
       <c r="D93">
-        <v>0.7681210643854236</v>
+        <v>0.7256118966709827</v>
       </c>
       <c r="E93">
-        <v>1.042269179560916</v>
+        <v>1.032179201632103</v>
       </c>
       <c r="F93">
-        <v>88450.38531118227</v>
+        <v>64497.72399666951</v>
       </c>
       <c r="G93">
-        <v>70.11053466796875</v>
+        <v>100.1855850219727</v>
       </c>
       <c r="H93">
-        <v>0.08626562356948853</v>
+        <v>0.1041076704859734</v>
       </c>
       <c r="I93">
-        <v>0.0009889309294521809</v>
+        <v>0.001240190234966576</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94">
-        <v>102.095011295625</v>
+        <v>85.52104401336446</v>
       </c>
       <c r="B94">
-        <v>0.1057859839209774</v>
+        <v>0.1238056694934646</v>
       </c>
       <c r="C94">
-        <v>0.0009690215073387984</v>
+        <v>0.001103549386777913</v>
       </c>
       <c r="D94">
-        <v>0.6965600237800346</v>
+        <v>0.6968131174346016</v>
       </c>
       <c r="E94">
-        <v>1.031910839476658</v>
+        <v>1.031507631998229</v>
       </c>
       <c r="F94">
-        <v>78793.81524920063</v>
+        <v>69399.99343271909</v>
       </c>
       <c r="G94">
-        <v>100.565185546875</v>
+        <v>111.2007141113281</v>
       </c>
       <c r="H94">
-        <v>0.1065004914999008</v>
+        <v>0.108015388250351</v>
       </c>
       <c r="I94">
-        <v>0.0009728235309012234</v>
+        <v>0.001097650150768459</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95">
-        <v>94.25461707635554</v>
+        <v>120.9422985057106</v>
       </c>
       <c r="B95">
-        <v>0.07705153857421826</v>
+        <v>0.09440400075014491</v>
       </c>
       <c r="C95">
-        <v>0.001040707600886504</v>
+        <v>0.00101736395741853</v>
       </c>
       <c r="D95">
-        <v>0.7676427887122367</v>
+        <v>0.70198168743117</v>
       </c>
       <c r="E95">
-        <v>1.037787604122255</v>
+        <v>1.032165905553469</v>
       </c>
       <c r="F95">
-        <v>82853.09738367423</v>
+        <v>75343.26803619425</v>
       </c>
       <c r="G95">
-        <v>94.56720733642578</v>
+        <v>108.1004333496094</v>
       </c>
       <c r="H95">
-        <v>0.07753278315067291</v>
+        <v>0.1018955931067467</v>
       </c>
       <c r="I95">
-        <v>0.001039185444824398</v>
+        <v>0.00101809948682785</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96">
-        <v>101.4510316236255</v>
+        <v>71.99827759280177</v>
       </c>
       <c r="B96">
-        <v>0.128553032105112</v>
+        <v>0.1031246966015183</v>
       </c>
       <c r="C96">
-        <v>0.001072701548420233</v>
+        <v>0.000882667818608427</v>
       </c>
       <c r="D96">
-        <v>0.6727593419467991</v>
+        <v>0.7260606670824068</v>
       </c>
       <c r="E96">
-        <v>1.030008326803699</v>
+        <v>1.037537472917495</v>
       </c>
       <c r="F96">
-        <v>68213.19844987047</v>
+        <v>92439.43583313809</v>
       </c>
       <c r="G96">
-        <v>102.96923828125</v>
+        <v>72.28475189208984</v>
       </c>
       <c r="H96">
-        <v>0.127612516283989</v>
+        <v>0.1032285466790199</v>
       </c>
       <c r="I96">
-        <v>0.001074862782843411</v>
+        <v>0.0008806199766695499</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97">
-        <v>91.9059926236006</v>
+        <v>127.5389633118084</v>
       </c>
       <c r="B97">
-        <v>0.1259536722314404</v>
+        <v>0.08629916605636875</v>
       </c>
       <c r="C97">
-        <v>0.0009989077394577661</v>
+        <v>0.001298777350797204</v>
       </c>
       <c r="D97">
-        <v>0.6792911646912159</v>
+        <v>0.7401669375814242</v>
       </c>
       <c r="E97">
-        <v>1.030786920040291</v>
+        <v>1.032374589261583</v>
       </c>
       <c r="F97">
-        <v>74376.66473446178</v>
+        <v>62364.36633244278</v>
       </c>
       <c r="G97">
-        <v>96.50450897216797</v>
+        <v>116.0914840698242</v>
       </c>
       <c r="H97">
-        <v>0.1225205808877945</v>
+        <v>0.09048361331224442</v>
       </c>
       <c r="I97">
-        <v>0.001001460012048483</v>
+        <v>0.001291756285354495</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98">
-        <v>81.43401489640408</v>
+        <v>91.32213090831578</v>
       </c>
       <c r="B98">
-        <v>0.09350781631387996</v>
+        <v>0.09732664896700162</v>
       </c>
       <c r="C98">
-        <v>0.001220073125955457</v>
+        <v>0.0009173134353636336</v>
       </c>
       <c r="D98">
-        <v>0.7555045872490377</v>
+        <v>0.7178954825409268</v>
       </c>
       <c r="E98">
-        <v>1.036564751376879</v>
+        <v>1.034212867037765</v>
       </c>
       <c r="F98">
-        <v>69426.26271102778</v>
+        <v>86740.4896913246</v>
       </c>
       <c r="G98">
-        <v>80.48849487304688</v>
+        <v>108.1237564086914</v>
       </c>
       <c r="H98">
-        <v>0.09383510053157806</v>
+        <v>0.08750529587268829</v>
       </c>
       <c r="I98">
-        <v>0.001219560042954981</v>
+        <v>0.0009092445834539831</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99">
-        <v>71.14737384692138</v>
+        <v>91.40241342415257</v>
       </c>
       <c r="B99">
-        <v>0.08453071564756513</v>
+        <v>0.09410281212277592</v>
       </c>
       <c r="C99">
-        <v>0.001076640853717171</v>
+        <v>0.0009823893695283456</v>
       </c>
       <c r="D99">
-        <v>0.7734461820242966</v>
+        <v>0.7306129590771383</v>
       </c>
       <c r="E99">
-        <v>1.042534473336286</v>
+        <v>1.034640524529086</v>
       </c>
       <c r="F99">
-        <v>82150.53498010209</v>
+        <v>82609.74492645131</v>
       </c>
       <c r="G99">
-        <v>69.58469390869141</v>
+        <v>105.1460952758789</v>
       </c>
       <c r="H99">
-        <v>0.0858614444732666</v>
+        <v>0.0864746943116188</v>
       </c>
       <c r="I99">
-        <v>0.001079394249245524</v>
+        <v>0.000977218383923173</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100">
-        <v>101.0889888274705</v>
+        <v>70.97971016102247</v>
       </c>
       <c r="B100">
-        <v>0.08502389277121437</v>
+        <v>0.08490480790497827</v>
       </c>
       <c r="C100">
-        <v>0.0009408567695833119</v>
+        <v>0.000926947104954077</v>
       </c>
       <c r="D100">
-        <v>0.7333281649475308</v>
+        <v>0.7644000309556259</v>
       </c>
       <c r="E100">
-        <v>1.035030249338583</v>
+        <v>1.042640582278119</v>
       </c>
       <c r="F100">
-        <v>86476.24464443262</v>
+        <v>94261.78920881344</v>
       </c>
       <c r="G100">
-        <v>109.2717590332031</v>
+        <v>70.90176391601562</v>
       </c>
       <c r="H100">
-        <v>0.08072251081466675</v>
+        <v>0.08462376892566681</v>
       </c>
       <c r="I100">
-        <v>0.0009408763726241887</v>
+        <v>0.00093222432769835</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101">
-        <v>120.5666117610905</v>
+        <v>81.11393951417104</v>
       </c>
       <c r="B101">
-        <v>0.09900361211214354</v>
+        <v>0.1003519830295185</v>
       </c>
       <c r="C101">
-        <v>0.0009500150541452265</v>
+        <v>0.001287716157601275</v>
       </c>
       <c r="D101">
-        <v>0.6843623944747705</v>
+        <v>0.7459933583562693</v>
       </c>
       <c r="E101">
-        <v>1.031939768405494</v>
+        <v>1.035269085127249</v>
       </c>
       <c r="F101">
-        <v>78483.88731377682</v>
+        <v>64665.23599851636</v>
       </c>
       <c r="G101">
-        <v>103.7344131469727</v>
+        <v>81.36767578125</v>
       </c>
       <c r="H101">
-        <v>0.1112709417939186</v>
+        <v>0.1005188301205635</v>
       </c>
       <c r="I101">
-        <v>0.00095280323876068</v>
+        <v>0.00128034153021872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>